<commit_message>
Atualização com bot para postagem automática no twitter
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_posts_devto.xlsx
+++ b/relatorios/relatorio_posts_devto.xlsx
@@ -13,7 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gráfico Tags" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$I$82</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -542,7 +542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -552,13 +552,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="5" customWidth="1" min="1" max="1"/>
-    <col width="124" customWidth="1" min="2" max="2"/>
-    <col width="29" customWidth="1" min="3" max="3"/>
-    <col width="132" customWidth="1" min="4" max="4"/>
+    <col width="118" customWidth="1" min="2" max="2"/>
+    <col width="38" customWidth="1" min="3" max="3"/>
+    <col width="134" customWidth="1" min="4" max="4"/>
     <col width="21" customWidth="1" min="5" max="5"/>
-    <col width="74" customWidth="1" min="6" max="6"/>
+    <col width="76" customWidth="1" min="6" max="6"/>
     <col width="9" customWidth="1" min="7" max="7"/>
     <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="21" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -602,6 +603,11 @@
           <t>comentarios</t>
         </is>
       </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>data_postagem</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="n">
@@ -623,7 +629,7 @@
         </is>
       </c>
       <c r="E2" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
@@ -631,10 +637,13 @@
         </is>
       </c>
       <c r="G2" s="4" t="n">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>45813.66982638889</v>
       </c>
     </row>
     <row r="3">
@@ -657,7 +666,7 @@
         </is>
       </c>
       <c r="E3" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
@@ -665,10 +674,13 @@
         </is>
       </c>
       <c r="G3" s="4" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>45814.61149305556</v>
       </c>
     </row>
     <row r="4">
@@ -677,31 +689,36 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>Resurgence of Software Design in 2025?</t>
+          <t>It's a DONUT!</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>Augusts Bautra</t>
+          <t>Niko from Axrisi</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/epigene/resurgence-of-software-design-in-2025-af3</t>
+          <t>https://dev.to/axrisi/its-a-donut-3gkk</t>
         </is>
       </c>
       <c r="E4" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>#software, #design</t>
+          <t>#frontendchallenge, #devchallenge, #css</t>
         </is>
       </c>
       <c r="G4" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H4" s="4" t="inlineStr"/>
+        <v>9</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>45814.74244212963</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">
@@ -709,31 +726,36 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Trying to get s*** done with an LLM</t>
+          <t>Start with DevOps in 3 simple steps 🐳</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>Sebastian Schürmann</t>
+          <t>Lara Stewart - DevOps Cloud Engineer</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/sebs/trying-to-get-s-done-with-an-llm-k05</t>
+          <t>https://dev.to/larastewart_engdev/start-with-devops-in-3-simple-steps-2lli</t>
         </is>
       </c>
       <c r="E5" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>#programming, #ai, #openapi</t>
+          <t>#productivity, #devops, #certification, #programming</t>
         </is>
       </c>
       <c r="G5" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>45815.62149305556</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
@@ -741,31 +763,36 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>My Wins of the Week! ⭐</t>
+          <t>Trying to get s*** done with an LLM</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>Anita Olsen</t>
+          <t>Sebastian Schürmann</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/anitaolsen/my-wins-of-the-week-58d6</t>
+          <t>https://dev.to/sebs/trying-to-get-s-done-with-an-llm-k05</t>
         </is>
       </c>
       <c r="E6" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>#weeklyretro</t>
+          <t>#programming, #ai, #openapi</t>
         </is>
       </c>
       <c r="G6" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="H6" s="4" t="inlineStr"/>
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>45814.68435185185</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="n">
@@ -773,32 +800,35 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>It's a DONUT!</t>
+          <t>QueerStation - A Digital Pride Zine Revolution</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>Niko from Axrisi</t>
+          <t>Sneha Das</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/axrisi/its-a-donut-3gkk</t>
+          <t>https://dev.to/sneha_2004/queerstation-a-digital-pride-zine-revolution-43h4</t>
         </is>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t>#frontendchallenge, #devchallenge, #css</t>
+          <t>#frontendchallenge, #devchallenge, #css, #webdev</t>
         </is>
       </c>
       <c r="G7" s="4" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>45815.31511574074</v>
       </c>
     </row>
     <row r="8">
@@ -807,32 +837,35 @@
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>I replaced the HTMX in the project to this module🔥</t>
+          <t>Top 10 VS Code Extensions for Enterprise Developers to Amp Up the Productivity</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>Anthony Max</t>
+          <t>Pankaj Singh</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/anthonymax/i-replaced-the-htmx-in-the-project-to-this-module-56bc</t>
+          <t>https://dev.to/pankaj_singh_1022ee93e755/top-10-vs-code-extensions-for-enterprise-developers-to-amp-up-the-productivity-n2n</t>
         </is>
       </c>
       <c r="E8" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>#webdev, #javascript, #programming, #opensource</t>
+          <t>#webdev, #programming, #vscode, #devops</t>
         </is>
       </c>
       <c r="G8" s="4" t="n">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>45815.58032407407</v>
       </c>
     </row>
     <row r="9">
@@ -841,32 +874,33 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>Bright Data Real-Time AI Agents Challenge Winner Announcement Delay</t>
+          <t>Resurgence of Software Design in 2025?</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>Jess Lee</t>
+          <t>Augusts Bautra</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/devteam/bright-data-real-time-ai-agents-challenge-winner-announcement-delay-21a0</t>
+          <t>https://dev.to/epigene/resurgence-of-software-design-in-2025-af3</t>
         </is>
       </c>
       <c r="E9" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t>#brightdatachallenge, #devchallenge</t>
+          <t>#software, #design</t>
         </is>
       </c>
       <c r="G9" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="H9" s="4" t="inlineStr"/>
+      <c r="I9" s="5" t="n">
+        <v>45814.6530787037</v>
       </c>
     </row>
     <row r="10">
@@ -875,31 +909,34 @@
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>Runner H Viral Content Factory Agent</t>
+          <t>My Wins of the Week! ⭐</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>Niko from Axrisi</t>
+          <t>Anita Olsen</t>
         </is>
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/axrisi/runner-h-viral-content-factory-agent-chn</t>
+          <t>https://dev.to/anitaolsen/my-wins-of-the-week-58d6</t>
         </is>
       </c>
       <c r="E10" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>#devchallenge, #runnerhchallenge, #ai, #machinelearning</t>
+          <t>#weeklyretro</t>
         </is>
       </c>
       <c r="G10" s="4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H10" s="4" t="inlineStr"/>
+      <c r="I10" s="5" t="n">
+        <v>45814.62424768518</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n">
@@ -907,32 +944,35 @@
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>Beyond Code: What 📖The Pragmatic Programmer Taught Me in One Chapter</t>
+          <t>🏠 Mailo: AI Email Replies, Seamlessly Delivered</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>PatrickBastosDeveloper</t>
+          <t>Sai Shravan Vadla</t>
         </is>
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/patrickbastosdeveloper/beyond-code-what-the-pragmatic-programmer-taught-me-in-one-chapter-8m3</t>
+          <t>https://dev.to/shravzzv/mailo-ai-email-replies-seamlessly-delivered-2lg6</t>
         </is>
       </c>
       <c r="E11" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F11" s="4" t="inlineStr">
         <is>
-          <t>#thepragmaticprogrammer, #books, #webdev</t>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
         </is>
       </c>
       <c r="G11" s="4" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>45815.42074074074</v>
       </c>
     </row>
     <row r="12">
@@ -941,31 +981,34 @@
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>Auto-Generating Clips for Social Media from Live Streams with the Strands Agents SDK</t>
+          <t>IoT Architectures Under Pressure: Smart Thermostat, Hardware (Part 7)</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>Todd Sharp</t>
+          <t>Adriano Repetti</t>
         </is>
       </c>
       <c r="D12" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/aws/auto-generating-clips-for-social-media-from-live-streams-with-the-strands-agents-sdk-1kkj</t>
+          <t>https://dev.to/adriano-repetti/iot-architectures-under-pressure-smart-thermostat-hardware-part-7-45c0</t>
         </is>
       </c>
       <c r="E12" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>#aws, #amazonivs, #livestreaming, #strandsagents</t>
+          <t>#iot, #diy, #c, #atmel</t>
         </is>
       </c>
       <c r="G12" s="4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H12" s="4" t="inlineStr"/>
+      <c r="I12" s="5" t="n">
+        <v>45815.59347222222</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n">
@@ -973,31 +1016,34 @@
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>5 Tips for Running Remote Dev Teams Remotely (with Teamcamp as Your Hub)</t>
+          <t>Biggest AI Scam: Builder.ai in the Spotlight</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>Pratham naik</t>
+          <t>Grenish rai</t>
         </is>
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/teamcamp/5-battle-tested-strategies-for-managing-remote-dev-teams-without-losing-your-sanity-3ka6</t>
+          <t>https://dev.to/grenishrai/legit-ai-says-builderio-1lkk</t>
         </is>
       </c>
       <c r="E13" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>#webdev, #productivity, #devops, #opensource</t>
+          <t>#news, #ai</t>
         </is>
       </c>
       <c r="G13" s="4" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="H13" s="4" t="inlineStr"/>
+      <c r="I13" s="5" t="n">
+        <v>45815.59521990741</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="n">
@@ -1005,32 +1051,33 @@
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>10 Cool CodePen Demos (May 2025)</t>
+          <t>🔹 Part 3: Terminal, Zen Mode, Extensions &amp; Hidden VS Code Gems (Windows &amp; Mac)!!</t>
         </is>
       </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
-          <t>Alvaro Montoro</t>
+          <t>Nishkarsh Pandey</t>
         </is>
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/alvaromontoro/10-cool-codepen-demos-may-2025-557d</t>
+          <t>https://dev.to/nish2005karsh/part-3-terminal-zen-mode-extensions-hidden-vs-code-gems-windows-mac-3eie</t>
         </is>
       </c>
       <c r="E14" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>#showdev, #html, #css, #javascript</t>
+          <t>#vscode, #programming, #cli, #terminal</t>
         </is>
       </c>
       <c r="G14" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="H14" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H14" s="4" t="inlineStr"/>
+      <c r="I14" s="5" t="n">
+        <v>45815.61939814815</v>
       </c>
     </row>
     <row r="15">
@@ -1039,31 +1086,34 @@
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>An awesome event to get hands on experience with the Google Workspace Developer Relations team. Check it out and register!</t>
+          <t>LEDGR - Receipts In, Insights Out. Automatically.</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Justin Poehnelt</t>
+          <t>Ayesha Imran</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/jpoehnelt/an-awesome-event-to-get-hands-on-experience-with-the-google-workspace-developer-relations-team-2em</t>
+          <t>https://dev.to/ayesha_imr/ledgr-receipts-in-insights-out-automatically-4ek2</t>
         </is>
       </c>
       <c r="E15" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>#appsheet, #appsscript, #googleworkspace, #google</t>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
         </is>
       </c>
       <c r="G15" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H15" s="4" t="inlineStr"/>
+      <c r="I15" s="5" t="n">
+        <v>45815.50930555556</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="n">
@@ -1071,31 +1121,34 @@
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>A Day at AWS Summit Hamburg 🇩🇪 – Innovation, AI, and Unforgettable Experiences</t>
+          <t>Access an EC2 Instance Using Session Manager (Even Without SSH Keys</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
-          <t>Ahmed Zeno</t>
+          <t>Samuel Ajisafe</t>
         </is>
       </c>
       <c r="D16" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/jadzeino/a-day-at-aws-summit-hamburg-innovation-ai-and-unforgettable-experiences-dpn</t>
+          <t>https://dev.to/sammy_cloud/access-an-ec2-instance-using-session-manager-even-without-ssh-keys-la1</t>
         </is>
       </c>
       <c r="E16" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>#aws, #ai, #hamburg, #webdev</t>
+          <t>Sem tags</t>
         </is>
       </c>
       <c r="G16" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="4" t="inlineStr"/>
+      <c r="I16" s="5" t="n">
+        <v>45815.62516203704</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="n">
@@ -1103,31 +1156,34 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>Security news weekly round-up - 6th June 2025</t>
+          <t>Auto-Invest: What’s Under the Hood?</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
         <is>
-          <t>Habdul Hazeez</t>
+          <t>Kaan Kaya</t>
         </is>
       </c>
       <c r="D17" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/ziizium/security-news-weekly-round-up-6th-june-2025-4118</t>
+          <t>https://dev.to/kaankaya/auto-invest-whats-under-the-hood-23kp</t>
         </is>
       </c>
       <c r="E17" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F17" s="4" t="inlineStr">
         <is>
-          <t>#security</t>
+          <t>#blockchain, #cryptocurrency, #web3, #dev</t>
         </is>
       </c>
       <c r="G17" s="4" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H17" s="4" t="inlineStr"/>
+      <c r="I17" s="5" t="n">
+        <v>45815.47560185185</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="n">
@@ -1135,31 +1191,34 @@
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>🚀 Mastering select_for_update() in Django: Prevent Race Conditions the Right Way</t>
+          <t>C++ in Embedded Systems: Modern Practices for Resource-Constrained Environments</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>karaa</t>
+          <t>Ethrynto</t>
         </is>
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/karaa1122/mastering-selectforupdate-in-django-prevent-race-conditions-the-right-way-4l56</t>
+          <t>https://dev.to/ethrynto/c-in-embedded-systems-modern-practices-for-resource-constrained-environments-412l</t>
         </is>
       </c>
       <c r="E18" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>#django, #api, #programming, #tutorial</t>
+          <t>#programming, #cpp, #coding</t>
         </is>
       </c>
       <c r="G18" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="4" t="inlineStr"/>
+      <c r="I18" s="5" t="n">
+        <v>45815.63618055556</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="n">
@@ -1167,31 +1226,34 @@
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Getting Started with Dependency Management in Rust Using Cargo.toml</t>
+          <t>✅ The Real Role of Software Testing: It’s More Than Bug Hunting</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>Rijul Rajesh</t>
+          <t>Vaibhav Kulshrestha</t>
         </is>
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/rijultp/getting-started-with-dependency-management-in-rust-using-cargotoml-54oo</t>
+          <t>https://dev.to/vaibhavkuls/the-real-role-of-software-testing-its-more-than-bug-hunting-22oa</t>
         </is>
       </c>
       <c r="E19" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F19" s="4" t="inlineStr">
         <is>
-          <t>#rust, #cargo, #language, #beginners</t>
+          <t>Sem tags</t>
         </is>
       </c>
       <c r="G19" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="4" t="inlineStr"/>
+      <c r="I19" s="5" t="n">
+        <v>45815.63219907408</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="n">
@@ -1199,31 +1261,34 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>Learning Perl – Introduction</t>
+          <t>Working with the Core FS Interface: Files, Directories, and Basic Operations (2/9)</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>LNATION</t>
+          <t>Rez Moss</t>
         </is>
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/lnation/learning-perl-introduction-3d1a</t>
+          <t>https://dev.to/rezmoss/working-with-the-core-fs-interface-files-directories-and-basic-operations-29-2mfj</t>
         </is>
       </c>
       <c r="E20" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>#perl, #beginners, #programming, #tutorial</t>
+          <t>#programming, #go, #softwaredevelopment, #systems</t>
         </is>
       </c>
       <c r="G20" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H20" s="4" t="inlineStr"/>
+      <c r="I20" s="5" t="n">
+        <v>45815.6375</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n">
@@ -1231,31 +1296,34 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>How I Got Cited by ChatGPT, Perplexity, and Grok — Without Gaming the System</t>
+          <t>Python Trending Weekly #105: Dify Breaks 100K Stars, Full-Stack Development Best Practices for 2025</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>Mayra Silva</t>
+          <t>PythonCat</t>
         </is>
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/blackblocksheep/how-i-got-cited-by-chatgpt-perplexity-and-grok-without-gaming-the-system-fg1</t>
+          <t>https://dev.to/pythoncat/python-trending-weekly-105-dify-breaks-100k-stars-full-stack-development-best-practices-for-2025-1ikp</t>
         </is>
       </c>
       <c r="E21" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F21" s="4" t="inlineStr">
         <is>
-          <t>#ai</t>
+          <t>#webdev, #programming, #ai, #python</t>
         </is>
       </c>
       <c r="G21" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H21" s="4" t="inlineStr"/>
+      <c r="I21" s="5" t="n">
+        <v>45815.62243055556</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="n">
@@ -1263,31 +1331,34 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>Building YAP’s Community: How I’m Leading the Charge and Why I’m the Best Fit</t>
+          <t>Inbox-as-Art Voice-Powered AI Art &amp; Email Creativity Postmark Challenge</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Christian</t>
+          <t>Edun Yusuf Aderogba</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/yaptech/building-yaps-community-how-im-leading-the-charge-and-why-im-the-best-fit-26d5</t>
+          <t>https://dev.to/volde/inbox-as-art-voice-powered-ai-art-email-creativity-postmark-challenge-32mh</t>
         </is>
       </c>
       <c r="E22" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>#edtech, #blockchain, #learning, #founder</t>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
         </is>
       </c>
       <c r="G22" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H22" s="4" t="inlineStr"/>
+      <c r="I22" s="5" t="n">
+        <v>45815.59050925926</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n">
@@ -1295,31 +1366,34 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Day 1 of getting my extension to 1,000 users</t>
+          <t>The "Idea Forge": An Autonomous Startup Idea Validator</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Arzuno</t>
+          <t>Taki Tajwaruzzaman Khan</t>
         </is>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/arzuno/day-1-of-getting-my-extension-to-1000-users-42np</t>
+          <t>https://dev.to/takitajwar17/the-idea-forge-an-autonomous-startup-idea-validator-5g82</t>
         </is>
       </c>
       <c r="E23" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F23" s="4" t="inlineStr">
         <is>
-          <t>#webdev, #programming, #javascript, #ai</t>
+          <t>#devchallenge, #runnerhchallenge, #ai, #machinelearning</t>
         </is>
       </c>
       <c r="G23" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H23" s="4" t="inlineStr"/>
+      <c r="I23" s="5" t="n">
+        <v>45815.61340277778</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="n">
@@ -1327,31 +1401,34 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Integrando Podcasts a Kiu: Cómo Construí un Agente Virtual Serverless con AWS Bedrock y Pinecone</t>
+          <t>Writing Scalable &amp; Maintainable Unit Tests in Django — A Practical Guide with Real Examples</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>Fernando Silva T</t>
+          <t>Shreyash Mishra</t>
         </is>
       </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/fernandosilvot/integrando-podcasts-a-kiu-como-construi-un-agente-virtual-serverless-con-aws-bedrock-y-pinecone-3l6e</t>
+          <t>https://dev.to/shreyash_jhon_doe/writing-scalable-maintainable-unit-tests-in-django-a-practical-guide-with-real-examples-47a4</t>
         </is>
       </c>
       <c r="E24" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>Sem tags</t>
+          <t>#webdev, #python, #django, #programming</t>
         </is>
       </c>
       <c r="G24" s="4" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="4" t="inlineStr"/>
+      <c r="I24" s="5" t="n">
+        <v>45815.61986111111</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="n">
@@ -1359,21 +1436,21 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Unified Cloud &amp; Shell Automation with pygcli</t>
+          <t>"Automate Your Design Job Hunt with Runner H – Daily Email Reports Made Easy"</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>Raghava Chellu</t>
+          <t>henry_68930cc9</t>
         </is>
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/raghavachellu/unified-cloud-shell-automation-with-pygcli-14go</t>
+          <t>https://dev.to/member_68930cc9/automate-your-design-job-hunt-with-runner-h-daily-email-reports-made-easy-19ig</t>
         </is>
       </c>
       <c r="E25" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.52920138889</v>
       </c>
       <c r="F25" s="4" t="inlineStr">
         <is>
@@ -1384,169 +1461,2023 @@
         <v>0</v>
       </c>
       <c r="H25" s="4" t="inlineStr"/>
+      <c r="I25" s="5" t="n">
+        <v>45815.61957175926</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>Why Developers Should Learn Linux (Even Just a Little)</t>
+          <t>InboxOps – AI-Powered Email Automation Platform Using Postmark Inbound Parsing</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
-          <t>Daniel | Frontend developer</t>
+          <t>Mihir Amin</t>
         </is>
       </c>
       <c r="D26" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/0xdaniiel/why-developers-should-learn-linux-even-just-a-little-3ig</t>
+          <t>https://dev.to/dynamicmortal/inboxops-ai-powered-email-automation-platform-using-postmark-inbound-parsing-1378</t>
         </is>
       </c>
       <c r="E26" s="5" t="n">
-        <v>45814.79509259259</v>
+        <v>45815.54785879629</v>
       </c>
       <c r="F26" s="4" t="inlineStr">
         <is>
-          <t>#linux, #productivity, #terminal, #programming</t>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
         </is>
       </c>
       <c r="G26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="H26" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="I26" s="5" t="n">
+        <v>45815.42284722222</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="n">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>Your Bundle is Lying to You: Hidden Costs of Tree-Shaking</t>
+          <t>🎵 I Built the World's First Email Music Studio with Postmark</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>Abhinav Shinoy</t>
+          <t>Lexeur</t>
         </is>
       </c>
       <c r="D27" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/abhinavshinoy90/your-bundle-is-lying-to-you-hidden-costs-of-tree-shaking-15pd</t>
+          <t>https://dev.to/1exer22/i-built-the-worlds-first-email-music-studio-with-postmark-l9l</t>
         </is>
       </c>
       <c r="E27" s="5" t="n">
-        <v>45814.80099537037</v>
+        <v>45815.54785879629</v>
       </c>
       <c r="F27" s="4" t="inlineStr">
         <is>
-          <t>#webdev, #webperf, #javascript, #frontend</t>
+          <t>#postmarkchallenge, #javascript, #vue, #firebase</t>
         </is>
       </c>
       <c r="G27" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="4" t="inlineStr"/>
+      <c r="I27" s="5" t="n">
+        <v>45815.65857638889</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="n">
-        <v>286</v>
+        <v>41</v>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>Bullet Summarization - Postmark Challenge</t>
+          <t>CRUD with JavaScript Fetch and the Platzi Fake Store API</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
         <is>
-          <t>Alin Pisica</t>
+          <t>Ahmed Niazy</t>
         </is>
       </c>
       <c r="D28" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/alinp25/bullet-summarization-postmark-challenge-1ggl</t>
+          <t>https://dev.to/ahmed_niazy/crud-with-javascript-fetch-and-the-platzi-fake-store-api-142e</t>
         </is>
       </c>
       <c r="E28" s="5" t="n">
-        <v>45814.8128125</v>
+        <v>45815.54785879629</v>
       </c>
       <c r="F28" s="4" t="inlineStr">
         <is>
-          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+          <t>#api, #javascript, #react, #vue</t>
         </is>
       </c>
       <c r="G28" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H28" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="H28" s="4" t="inlineStr"/>
+      <c r="I28" s="5" t="n">
+        <v>45815.56478009259</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="n">
-        <v>289</v>
+        <v>43</v>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>InvisiBox: Bi-directional privacy-first communication channel for workplaces.</t>
+          <t>Whats the difference b/w Path and Query in FastAPI?</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>sahra 💫</t>
+          <t>Sarvesh Kesharwani</t>
         </is>
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/sarahokolo/invisibox-bi-directional-privacy-first-communication-channel-for-workplaces-cfp</t>
+          <t>https://dev.to/sarvesh42/whats-the-difference-bw-path-and-query-in-fastapi-1c3e</t>
         </is>
       </c>
       <c r="E29" s="5" t="n">
-        <v>45814.8128125</v>
+        <v>45815.54785879629</v>
       </c>
       <c r="F29" s="4" t="inlineStr">
         <is>
-          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+          <t>#machinelearning, #python, #fastapi, #programming</t>
         </is>
       </c>
       <c r="G29" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H29" s="4" t="inlineStr"/>
+      <c r="I29" s="5" t="n">
+        <v>45815.65221064815</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="n">
-        <v>290</v>
+        <v>45</v>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>From Zero to Arrays: Introducing My New Project</t>
+          <t>Never Get Blindsided by an Expired SSL Certificate: 6 Monitoring Services Compared</t>
         </is>
       </c>
       <c r="C30" s="4" t="inlineStr">
         <is>
-          <t>Genix</t>
+          <t>Riley Chen</t>
         </is>
       </c>
       <c r="D30" s="4" t="inlineStr">
         <is>
-          <t>https://dev.to/m__mdy__m/from-zero-to-arrays-introducing-my-new-project-5h9d</t>
+          <t>https://dev.to/rileychen/never-get-blindsided-by-an-expired-ssl-certificate-6-monitoring-services-compared-4ghi</t>
         </is>
       </c>
       <c r="E30" s="5" t="n">
-        <v>45814.8128125</v>
+        <v>45815.54785879629</v>
       </c>
       <c r="F30" s="4" t="inlineStr">
         <is>
-          <t>#discuss, #programming, #computerscience, #beginners</t>
+          <t>#webdev, #domains, #ssl, #uptime</t>
         </is>
       </c>
       <c r="G30" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4" t="inlineStr"/>
+      <c r="I30" s="5" t="n">
+        <v>45815.64118055555</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t>A Practical Guide to MLOps on AWS: Streaming Data Ingestion with Kinesis Firehose (Phase 01)</t>
+        </is>
+      </c>
+      <c r="C31" s="4" t="inlineStr">
+        <is>
+          <t>Mohsin Sheikhani</t>
+        </is>
+      </c>
+      <c r="D31" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/mohsinsheikhani/a-practical-guide-to-mlops-on-aws-streaming-data-ingestion-with-kinesis-firehose-phase-01-1bi7</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>45815.54785879629</v>
+      </c>
+      <c r="F31" s="4" t="inlineStr">
+        <is>
+          <t>#aws, #serverless, #mlops, #dataengineering</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4" t="inlineStr"/>
+      <c r="I31" s="5" t="n">
+        <v>45815.64299768519</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>How Missing Initialization of out Parameters Leads to Runtime Errors in C#</t>
+        </is>
+      </c>
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>boomi1</t>
+        </is>
+      </c>
+      <c r="D32" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/boomi1/how-missing-initialization-of-out-parameters-leads-to-runtime-errors-in-c-449j</t>
+        </is>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>45815.54785879629</v>
+      </c>
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>#csharp</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4" t="inlineStr"/>
+      <c r="I32" s="5" t="n">
+        <v>45815.64</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="n">
+        <v>48</v>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>Runner H "AI Agent Prompting" Challenge</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="inlineStr">
+        <is>
+          <t>Wael</t>
+        </is>
+      </c>
+      <c r="D33" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/waelel/runner-h-ai-agent-prompting-challenge-1jfk</t>
+        </is>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>45815.54785879629</v>
+      </c>
+      <c r="F33" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #runnerhchallenge, #ai, #machinelearning</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4" t="inlineStr"/>
+      <c r="I33" s="5" t="n">
+        <v>45815.64230324074</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="n">
+        <v>83</v>
+      </c>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t>CC-my-Jira: Agentic JIRA Ticketing via Postmark</t>
+        </is>
+      </c>
+      <c r="C34" s="4" t="inlineStr">
+        <is>
+          <t>Younes Laaroussi</t>
+        </is>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/youneslaaroussi/cc-my-jira-agentic-jira-ticketing-via-postmark-amf</t>
+        </is>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F34" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" s="5" t="n">
+        <v>45815.6784375</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="n">
+        <v>86</v>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>Indian AI model DESTROYS o3-mini, Google DeepSearch is open source, OpenAI's new models and TypeScript SDK, and more</t>
+        </is>
+      </c>
+      <c r="C35" s="4" t="inlineStr">
+        <is>
+          <t>This Week in AI Engineering</t>
+        </is>
+      </c>
+      <c r="D35" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/thisweekinaiengineering/indian-ai-model-destroys-o3-mini-google-deepsearch-is-open-source-openais-new-models-and-2ol1</t>
+        </is>
+      </c>
+      <c r="E35" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F35" s="4" t="inlineStr">
+        <is>
+          <t>#ai, #machinelearning, #programming, #beginners</t>
+        </is>
+      </c>
+      <c r="G35" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4" t="inlineStr"/>
+      <c r="I35" s="5" t="n">
+        <v>45815.70833333334</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="n">
+        <v>87</v>
+      </c>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t>The Definitive Guide to Digital Transformation</t>
+        </is>
+      </c>
+      <c r="C36" s="4" t="inlineStr">
+        <is>
+          <t>William Oliver</t>
+        </is>
+      </c>
+      <c r="D36" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/williamoliver/the-definitive-guide-to-digital-transformation-1p55</t>
+        </is>
+      </c>
+      <c r="E36" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F36" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4" t="inlineStr"/>
+      <c r="I36" s="5" t="n">
+        <v>45815.70333333333</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="n">
+        <v>88</v>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>💡You're Not Chatting With AI, You're Giving It a Job. Here's How</t>
+        </is>
+      </c>
+      <c r="C37" s="4" t="inlineStr">
+        <is>
+          <t>idavidov13</t>
+        </is>
+      </c>
+      <c r="D37" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/idavidov13/youre-not-chatting-with-ai-youre-giving-it-a-job-heres-how-1k3n</t>
+        </is>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F37" s="4" t="inlineStr">
+        <is>
+          <t>#ai, #chatgpt, #learning, #tutorial</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4" t="inlineStr"/>
+      <c r="I37" s="5" t="n">
+        <v>45815.70414351852</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="n">
+        <v>89</v>
+      </c>
+      <c r="B38" s="4" t="inlineStr">
+        <is>
+          <t>Debugging Memory Leaks in Node.js: A Complete Guide to heapdump, clinic.js, and v8-tools</t>
+        </is>
+      </c>
+      <c r="C38" s="4" t="inlineStr">
+        <is>
+          <t>Sarvesh</t>
+        </is>
+      </c>
+      <c r="D38" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/crit3cal/debugging-memory-leaks-in-nodejs-a-complete-guide-to-heapdump-clinicjs-and-v8-tools-19b</t>
+        </is>
+      </c>
+      <c r="E38" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F38" s="4" t="inlineStr">
+        <is>
+          <t>#security, #performance, #webperf, #node</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4" t="inlineStr"/>
+      <c r="I38" s="5" t="n">
+        <v>45815.70478009259</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="n">
+        <v>90</v>
+      </c>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>Learning Go Interface Encapsulation from K8s</t>
+        </is>
+      </c>
+      <c r="C39" s="4" t="inlineStr">
+        <is>
+          <t>Leapcell</t>
+        </is>
+      </c>
+      <c r="D39" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/leapcell/learning-go-interface-encapsulation-from-k8s-nnd</t>
+        </is>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F39" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #programming, #backend, #go</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H30" s="4" t="inlineStr"/>
+      <c r="H39" s="4" t="inlineStr"/>
+      <c r="I39" s="5" t="n">
+        <v>45815.67009259259</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="n">
+        <v>91</v>
+      </c>
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t>Java Full Stack Developer (Fresher)</t>
+        </is>
+      </c>
+      <c r="C40" s="4" t="inlineStr">
+        <is>
+          <t>Elayaraj C</t>
+        </is>
+      </c>
+      <c r="D40" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/elayaraj31/java-full-stack-developer-fresher-51gk</t>
+        </is>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F40" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G40" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4" t="inlineStr"/>
+      <c r="I40" s="5" t="n">
+        <v>45815.69957175926</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="n">
+        <v>92</v>
+      </c>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>✨ Building a Cosmic Note-Taking App: A Journey Through Space and Code</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="inlineStr">
+        <is>
+          <t>Arvin Jafary</t>
+        </is>
+      </c>
+      <c r="D41" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/arwinux/building-a-cosmic-note-taking-app-a-journey-through-space-and-code-3nlj</t>
+        </is>
+      </c>
+      <c r="E41" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F41" s="4" t="inlineStr">
+        <is>
+          <t>#javascript, #webdev, #tutorial, #css</t>
+        </is>
+      </c>
+      <c r="G41" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="4" t="inlineStr"/>
+      <c r="I41" s="5" t="n">
+        <v>45815.69543981482</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="B42" s="4" t="inlineStr">
+        <is>
+          <t>My Java Journey ☕</t>
+        </is>
+      </c>
+      <c r="C42" s="4" t="inlineStr">
+        <is>
+          <t>Jostin Soza</t>
+        </is>
+      </c>
+      <c r="D42" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jostin_soza_20/my-java-journey-m1</t>
+        </is>
+      </c>
+      <c r="E42" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #java, #beginners, #learning</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4" t="inlineStr"/>
+      <c r="I42" s="5" t="n">
+        <v>45815.69046296296</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="n">
+        <v>94</v>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>I Fixed My Slow Nginx + Gunicorn Setup — Here’s How It Became 3X Faster</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="inlineStr">
+        <is>
+          <t>Chimobi Roland</t>
+        </is>
+      </c>
+      <c r="D43" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/orc-1/i-fixed-my-slow-nginx-gunicorn-setup-heres-how-it-became-3x-faster-1j9f</t>
+        </is>
+      </c>
+      <c r="E43" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F43" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #nginx, #devops</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="4" t="inlineStr"/>
+      <c r="I43" s="5" t="n">
+        <v>45815.68766203704</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="n">
+        <v>95</v>
+      </c>
+      <c r="B44" s="4" t="inlineStr">
+        <is>
+          <t>Learning Perl - References</t>
+        </is>
+      </c>
+      <c r="C44" s="4" t="inlineStr">
+        <is>
+          <t>LNATION</t>
+        </is>
+      </c>
+      <c r="D44" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/lnation/learning-perl-references-3jfe</t>
+        </is>
+      </c>
+      <c r="E44" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F44" s="4" t="inlineStr">
+        <is>
+          <t>#perl, #beginners, #programming, #tutorial</t>
+        </is>
+      </c>
+      <c r="G44" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="4" t="inlineStr"/>
+      <c r="I44" s="5" t="n">
+        <v>45815.68759259259</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="n">
+        <v>96</v>
+      </c>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>SpotMyFile: AI-Powered File Search for Your PC</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="inlineStr">
+        <is>
+          <t>Rishabh Singh</t>
+        </is>
+      </c>
+      <c r="D45" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/rishabh705/spotmyfile-ai-powered-file-search-for-your-pc-5e6b</t>
+        </is>
+      </c>
+      <c r="E45" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F45" s="4" t="inlineStr">
+        <is>
+          <t>#python, #filesearch, #ai, #productivity</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4" t="inlineStr"/>
+      <c r="I45" s="5" t="n">
+        <v>45815.68017361111</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="n">
+        <v>97</v>
+      </c>
+      <c r="B46" s="4" t="inlineStr">
+        <is>
+          <t>Installing AWS CLI v2</t>
+        </is>
+      </c>
+      <c r="C46" s="4" t="inlineStr">
+        <is>
+          <t>DevOps Playground</t>
+        </is>
+      </c>
+      <c r="D46" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/devopsplayground/installing-aws-cli-v2-1cjh</t>
+        </is>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v>45815.59225694444</v>
+      </c>
+      <c r="F46" s="4" t="inlineStr">
+        <is>
+          <t>#devops, #aws, #awscli, #linux</t>
+        </is>
+      </c>
+      <c r="G46" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="4" t="inlineStr"/>
+      <c r="I46" s="5" t="n">
+        <v>45815.67925925926</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="n">
+        <v>104</v>
+      </c>
+      <c r="B47" s="4" t="inlineStr">
+        <is>
+          <t>CouponAI: Turn Promotional Emails into Smart Savings</t>
+        </is>
+      </c>
+      <c r="C47" s="4" t="inlineStr">
+        <is>
+          <t>Utkarsh212</t>
+        </is>
+      </c>
+      <c r="D47" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/utkarsh212/couponai-turn-promotional-emails-into-smart-savings-53dc</t>
+        </is>
+      </c>
+      <c r="E47" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F47" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H47" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I47" s="5" t="n">
+        <v>45815.7374537037</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="n">
+        <v>105</v>
+      </c>
+      <c r="B48" s="4" t="inlineStr">
+        <is>
+          <t>How Hard Can It Be? Building a Photo Sharing App Is Easy 😓</t>
+        </is>
+      </c>
+      <c r="C48" s="4" t="inlineStr">
+        <is>
+          <t>Lukas Mauser</t>
+        </is>
+      </c>
+      <c r="D48" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/wimadev/how-hard-can-it-be-building-a-photo-sharing-app-is-easy-19mo</t>
+        </is>
+      </c>
+      <c r="E48" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F48" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #programming, #javascript, #vue</t>
+        </is>
+      </c>
+      <c r="G48" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H48" s="4" t="inlineStr"/>
+      <c r="I48" s="5" t="n">
+        <v>45815.75832175926</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="n">
+        <v>108</v>
+      </c>
+      <c r="B49" s="4" t="inlineStr">
+        <is>
+          <t>How I Automated My Tech Blog Workflow Using Runner H and AI</t>
+        </is>
+      </c>
+      <c r="C49" s="4" t="inlineStr">
+        <is>
+          <t>Aditya</t>
+        </is>
+      </c>
+      <c r="D49" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/extinctsion/how-i-automated-my-tech-blog-workflow-using-runner-h-and-ai-4h4</t>
+        </is>
+      </c>
+      <c r="E49" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F49" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #runnerhchallenge, #ai, #machinelearning</t>
+        </is>
+      </c>
+      <c r="G49" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I49" s="5" t="n">
+        <v>45815.45103009259</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="n">
+        <v>111</v>
+      </c>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>10 Years on GitHub: What I’ve Learned</t>
+        </is>
+      </c>
+      <c r="C50" s="4" t="inlineStr">
+        <is>
+          <t>Mathias Falci</t>
+        </is>
+      </c>
+      <c r="D50" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/mathiasfc/10-years-on-github-what-ive-learned-4h8e</t>
+        </is>
+      </c>
+      <c r="E50" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F50" s="4" t="inlineStr">
+        <is>
+          <t>#github, #developers, #career, #programming</t>
+        </is>
+      </c>
+      <c r="G50" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H50" s="4" t="inlineStr"/>
+      <c r="I50" s="5" t="n">
+        <v>45815.75216435185</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="n">
+        <v>112</v>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>Step-by-Step: Build Your First RAG Chatbot Fast</t>
+        </is>
+      </c>
+      <c r="C51" s="4" t="inlineStr">
+        <is>
+          <t>Kabir Arora</t>
+        </is>
+      </c>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/startkabir/step-by-step-build-your-first-rag-chatbot-fast-3703</t>
+        </is>
+      </c>
+      <c r="E51" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F51" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #rag, #llm, #ai</t>
+        </is>
+      </c>
+      <c r="G51" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H51" s="4" t="inlineStr"/>
+      <c r="I51" s="5" t="n">
+        <v>45815.76041666666</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="n">
+        <v>115</v>
+      </c>
+      <c r="B52" s="4" t="inlineStr">
+        <is>
+          <t>🚀 I Built a Clean &amp; Modern Next.js E-commerce Template — And You Can Use It or Contribute!</t>
+        </is>
+      </c>
+      <c r="C52" s="4" t="inlineStr">
+        <is>
+          <t>Mohamed Ibrahim</t>
+        </is>
+      </c>
+      <c r="D52" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/moibra/i-built-a-clean-modern-nextjs-e-commerce-template-and-you-can-use-it-or-contribute-2d0i</t>
+        </is>
+      </c>
+      <c r="E52" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #programming, #javascript, #beginners</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="4" t="inlineStr"/>
+      <c r="I52" s="5" t="n">
+        <v>45815.7656712963</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="n">
+        <v>117</v>
+      </c>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t>Memory MCP with Semantic Search Support</t>
+        </is>
+      </c>
+      <c r="C53" s="4" t="inlineStr">
+        <is>
+          <t>Mehran</t>
+        </is>
+      </c>
+      <c r="D53" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/mehrant/-k1o</t>
+        </is>
+      </c>
+      <c r="E53" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F53" s="4" t="inlineStr">
+        <is>
+          <t>#cursor, #mcp, #programming, #ai</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="4" t="inlineStr"/>
+      <c r="I53" s="5" t="n">
+        <v>45815.7903125</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="n">
+        <v>118</v>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
+        <is>
+          <t>Testing Blog sync updated</t>
+        </is>
+      </c>
+      <c r="C54" s="4" t="inlineStr">
+        <is>
+          <t>Karthikeyan</t>
+        </is>
+      </c>
+      <c r="D54" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/imkarthikeyan/testing-blog-sync-updated-337j</t>
+        </is>
+      </c>
+      <c r="E54" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>#test, #firstpost, #writing</t>
+        </is>
+      </c>
+      <c r="G54" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="4" t="inlineStr"/>
+      <c r="I54" s="5" t="n">
+        <v>45815.77484953704</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="n">
+        <v>119</v>
+      </c>
+      <c r="B55" s="4" t="inlineStr">
+        <is>
+          <t>Ice Tea celebration in June</t>
+        </is>
+      </c>
+      <c r="C55" s="4" t="inlineStr">
+        <is>
+          <t>Ulrike Herold</t>
+        </is>
+      </c>
+      <c r="D55" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ulrikedetective/ice-tea-celebration-in-june-p7k</t>
+        </is>
+      </c>
+      <c r="E55" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F55" s="4" t="inlineStr">
+        <is>
+          <t>#frontendchallenge, #devchallenge, #css</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="4" t="inlineStr"/>
+      <c r="I55" s="5" t="n">
+        <v>45815.77486111111</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>Ever needed a bank-agnostic spend analyzer that is self-hostable?</t>
+        </is>
+      </c>
+      <c r="C56" s="4" t="inlineStr">
+        <is>
+          <t>Shriji</t>
+        </is>
+      </c>
+      <c r="D56" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/shriji/ever-needed-a-bank-agnostic-spend-analyzer-that-is-self-hostable-3p36</t>
+        </is>
+      </c>
+      <c r="E56" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G56" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="4" t="inlineStr"/>
+      <c r="I56" s="5" t="n">
+        <v>45815.77483796296</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="n">
+        <v>121</v>
+      </c>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t>PIDM — Python Internet Download Manager</t>
+        </is>
+      </c>
+      <c r="C57" s="4" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="D57" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ericluckson1999/pidm-python-internet-download-manager-4ak9</t>
+        </is>
+      </c>
+      <c r="E57" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F57" s="4" t="inlineStr">
+        <is>
+          <t>#download, #pidm, #programming, #python</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="4" t="inlineStr"/>
+      <c r="I57" s="5" t="n">
+        <v>45815.77880787037</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="n">
+        <v>122</v>
+      </c>
+      <c r="B58" s="4" t="inlineStr">
+        <is>
+          <t>Problem Solving Doesn’t Take a Break — Even on Eid-ul-Azha 2025</t>
+        </is>
+      </c>
+      <c r="C58" s="4" t="inlineStr">
+        <is>
+          <t>Mahmudul Haque Shawon</t>
+        </is>
+      </c>
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/mahmudulhaqueshawon/problem-solving-doesnt-take-a-break-even-on-eid-ul-azha-2025-4ajm</t>
+        </is>
+      </c>
+      <c r="E58" s="5" t="n">
+        <v>45815.67658564815</v>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="4" t="inlineStr"/>
+      <c r="I58" s="5" t="n">
+        <v>45815.77701388889</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="4" t="n">
+        <v>198</v>
+      </c>
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t>🪙 LEDGR: AI-Powered Expense Tracker | Email-to-Expense Magic with Postmark &amp; Gemini AI</t>
+        </is>
+      </c>
+      <c r="C59" s="4" t="inlineStr">
+        <is>
+          <t>Jackson Kasi</t>
+        </is>
+      </c>
+      <c r="D59" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jacksonkasi/ledgr-ai-powered-expense-tracker-email-to-expense-magic-with-postmark-gemini-ai-d2o</t>
+        </is>
+      </c>
+      <c r="E59" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F59" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G59" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H59" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I59" s="5" t="n">
+        <v>45816.62224537037</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="B60" s="4" t="inlineStr">
+        <is>
+          <t>Kubernetes Deployments vs StatefulSets</t>
+        </is>
+      </c>
+      <c r="C60" s="4" t="inlineStr">
+        <is>
+          <t>DevOps Daily</t>
+        </is>
+      </c>
+      <c r="D60" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/devopsdaily/kubernetes-deployments-vs-statefulsets-3m9b</t>
+        </is>
+      </c>
+      <c r="E60" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>#kubernetes, #devops, #docker, #beginners</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H60" s="4" t="inlineStr"/>
+      <c r="I60" s="5" t="n">
+        <v>45816.66914351852</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="4" t="n">
+        <v>201</v>
+      </c>
+      <c r="B61" s="4" t="inlineStr">
+        <is>
+          <t>Mission 5 Part One Meet for Coffee</t>
+        </is>
+      </c>
+      <c r="C61" s="4" t="inlineStr">
+        <is>
+          <t>Sarah Bartley-Dye</t>
+        </is>
+      </c>
+      <c r="D61" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/theoriginalbpc/mission-5-part-one-meet-for-coffee-2n6d</t>
+        </is>
+      </c>
+      <c r="E61" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F61" s="4" t="inlineStr">
+        <is>
+          <t>#cnc2018, #career, #careerdevelopment</t>
+        </is>
+      </c>
+      <c r="G61" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="4" t="inlineStr"/>
+      <c r="I61" s="5" t="n">
+        <v>45816.79103009259</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="4" t="n">
+        <v>202</v>
+      </c>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t>Inbox Translator: Automatic Email Translation Made Easy</t>
+        </is>
+      </c>
+      <c r="C62" s="4" t="inlineStr">
+        <is>
+          <t>Eunice</t>
+        </is>
+      </c>
+      <c r="D62" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/adonaitechnologies/inbox-translator-automatic-email-translation-made-easy-2hc7</t>
+        </is>
+      </c>
+      <c r="E62" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G62" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H62" s="4" t="inlineStr"/>
+      <c r="I62" s="5" t="n">
+        <v>45816.86697916667</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4" t="n">
+        <v>203</v>
+      </c>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t>Meilisearch Filters: A Hands-On Guide for Developers</t>
+        </is>
+      </c>
+      <c r="C63" s="4" t="inlineStr">
+        <is>
+          <t>Shrijith Venkatramana</t>
+        </is>
+      </c>
+      <c r="D63" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/shrsv/meilisearch-filters-a-hands-on-guide-for-developers-3bi5</t>
+        </is>
+      </c>
+      <c r="E63" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F63" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #beginners, #productivity, #tooling</t>
+        </is>
+      </c>
+      <c r="G63" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H63" s="4" t="inlineStr"/>
+      <c r="I63" s="5" t="n">
+        <v>45816.71057870371</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="n">
+        <v>204</v>
+      </c>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>Save Hours on API Testing: Auto-Generate Postman Collections from Your Express.js App 🧪</t>
+        </is>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>Ali nazari</t>
+        </is>
+      </c>
+      <c r="D64" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/silentwatcher_95/save-hours-on-api-testing-auto-generate-postman-collections-from-your-expressjs-app-mbo</t>
+        </is>
+      </c>
+      <c r="E64" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F64" s="4" t="inlineStr">
+        <is>
+          <t>#javascript, #node, #webdev, #programming</t>
+        </is>
+      </c>
+      <c r="G64" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H64" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I64" s="5" t="n">
+        <v>45816.77078703704</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="n">
+        <v>205</v>
+      </c>
+      <c r="B65" s="4" t="inlineStr">
+        <is>
+          <t>🌲 Git better at ignore-ing</t>
+        </is>
+      </c>
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>Himanshu</t>
+        </is>
+      </c>
+      <c r="D65" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/himanshuc3/git-better-at-ignore-ing-5cmf</t>
+        </is>
+      </c>
+      <c r="E65" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F65" s="4" t="inlineStr">
+        <is>
+          <t>#todayilearned, #git, #bash</t>
+        </is>
+      </c>
+      <c r="G65" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="4" t="inlineStr"/>
+      <c r="I65" s="5" t="n">
+        <v>45816.81711805556</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="n">
+        <v>206</v>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>StoryMail 🧠📬 – Your AI Inbox Detective</t>
+        </is>
+      </c>
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>ashish-nagmoti</t>
+        </is>
+      </c>
+      <c r="D66" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ashish_nagmoti/storymail-your-ai-inbox-detective-4c15</t>
+        </is>
+      </c>
+      <c r="E66" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F66" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G66" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H66" s="4" t="inlineStr"/>
+      <c r="I66" s="5" t="n">
+        <v>45816.77556712963</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="n">
+        <v>207</v>
+      </c>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>🚀 Just launched my new app: LinkList! 🔗📌</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>ssekabira robert sims</t>
+        </is>
+      </c>
+      <c r="D67" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ssekabirarobertsims/just-launched-my-new-app-linklist-8i0</t>
+        </is>
+      </c>
+      <c r="E67" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F67" s="4" t="inlineStr">
+        <is>
+          <t>#showdev, #productivity, #webdev, #mobile</t>
+        </is>
+      </c>
+      <c r="G67" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I67" s="5" t="n">
+        <v>45816.78409722223</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4" t="n">
+        <v>208</v>
+      </c>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>Visualizing GPU Metrics with DCGM Exporter</t>
+        </is>
+      </c>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>murajo</t>
+        </is>
+      </c>
+      <c r="D68" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/murajo/visualizing-gpu-metrics-with-dcgm-exporter-1268</t>
+        </is>
+      </c>
+      <c r="E68" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F68" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G68" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="4" t="inlineStr"/>
+      <c r="I68" s="5" t="n">
+        <v>45816.86724537037</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="4" t="n">
+        <v>209</v>
+      </c>
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t>My first experience with Arch Linux</t>
+        </is>
+      </c>
+      <c r="C69" s="4" t="inlineStr">
+        <is>
+          <t>Tenry</t>
+        </is>
+      </c>
+      <c r="D69" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/tenry/my-first-experience-with-arch-linux-3jh3</t>
+        </is>
+      </c>
+      <c r="E69" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F69" s="4" t="inlineStr">
+        <is>
+          <t>#archlinux</t>
+        </is>
+      </c>
+      <c r="G69" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="4" t="inlineStr"/>
+      <c r="I69" s="5" t="n">
+        <v>45816.85966435185</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4" t="n">
+        <v>210</v>
+      </c>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>Screw your favorite programming language</t>
+        </is>
+      </c>
+      <c r="C70" s="4" t="inlineStr">
+        <is>
+          <t>Dany Tulumidis</t>
+        </is>
+      </c>
+      <c r="D70" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/danytulumidis/screw-your-favorite-programming-language-40c0</t>
+        </is>
+      </c>
+      <c r="E70" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F70" s="4" t="inlineStr">
+        <is>
+          <t>#softwareenginner, #softwaredeveloper, #programming, #programminglanguages</t>
+        </is>
+      </c>
+      <c r="G70" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="4" t="inlineStr"/>
+      <c r="I70" s="5" t="n">
+        <v>45816.83085648148</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4" t="n">
+        <v>211</v>
+      </c>
+      <c r="B71" s="4" t="inlineStr">
+        <is>
+          <t>TrackLah!</t>
+        </is>
+      </c>
+      <c r="C71" s="4" t="inlineStr">
+        <is>
+          <t>Tan Yong He</t>
+        </is>
+      </c>
+      <c r="D71" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/tanyonghe/tracklah-9e9</t>
+        </is>
+      </c>
+      <c r="E71" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F71" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G71" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H71" s="4" t="inlineStr"/>
+      <c r="I71" s="5" t="n">
+        <v>45816.59214120371</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="4" t="n">
+        <v>212</v>
+      </c>
+      <c r="B72" s="4" t="inlineStr">
+        <is>
+          <t>Turbine seu Copilot no VS Code com MCP (Model Context Protocol)</t>
+        </is>
+      </c>
+      <c r="C72" s="4" t="inlineStr">
+        <is>
+          <t>Miquéias Telles</t>
+        </is>
+      </c>
+      <c r="D72" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/miqstelles/turbine-seu-copilot-no-vs-code-com-mcp-model-context-protocol-4lf7</t>
+        </is>
+      </c>
+      <c r="E72" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F72" s="4" t="inlineStr">
+        <is>
+          <t>#mcp, #githubcopilot, #ai, #programming</t>
+        </is>
+      </c>
+      <c r="G72" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" s="4" t="inlineStr"/>
+      <c r="I72" s="5" t="n">
+        <v>45816.85195601852</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="4" t="n">
+        <v>213</v>
+      </c>
+      <c r="B73" s="4" t="inlineStr">
+        <is>
+          <t>IncentiveBox: Your personal savings wallet</t>
+        </is>
+      </c>
+      <c r="C73" s="4" t="inlineStr">
+        <is>
+          <t>Shyam Sundar</t>
+        </is>
+      </c>
+      <c r="D73" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/shyamsravikumar/incentivebox-your-personal-savings-wallet-plb</t>
+        </is>
+      </c>
+      <c r="E73" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F73" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G73" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" s="4" t="inlineStr"/>
+      <c r="I73" s="5" t="n">
+        <v>45816.8478587963</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="4" t="n">
+        <v>214</v>
+      </c>
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t>Invisible Threads: Group email without the exposure</t>
+        </is>
+      </c>
+      <c r="C74" s="4" t="inlineStr">
+        <is>
+          <t>Josh Davis</t>
+        </is>
+      </c>
+      <c r="D74" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jdav-dev/invisible-threads-group-email-without-the-exposure-24n6</t>
+        </is>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F74" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G74" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" s="4" t="inlineStr"/>
+      <c r="I74" s="5" t="n">
+        <v>45816.84966435185</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="n">
+        <v>215</v>
+      </c>
+      <c r="B75" s="4" t="inlineStr">
+        <is>
+          <t>🚀 New Release: pyseoa v0.2.3</t>
+        </is>
+      </c>
+      <c r="C75" s="4" t="inlineStr">
+        <is>
+          <t>sempre76</t>
+        </is>
+      </c>
+      <c r="D75" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/huetteldorf/new-release-pyseoa-v023-1mco</t>
+        </is>
+      </c>
+      <c r="E75" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F75" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #python, #seo, #cli</t>
+        </is>
+      </c>
+      <c r="G75" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="4" t="inlineStr"/>
+      <c r="I75" s="5" t="n">
+        <v>45816.8561574074</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="4" t="n">
+        <v>216</v>
+      </c>
+      <c r="B76" s="4" t="inlineStr">
+        <is>
+          <t>Build Your CAN Bus Skills: A Beginner’s Guide to Using CAN in Your Projects</t>
+        </is>
+      </c>
+      <c r="C76" s="4" t="inlineStr">
+        <is>
+          <t>Ganesh Kumar</t>
+        </is>
+      </c>
+      <c r="D76" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ganesh-kumar/build-your-can-bus-skills-a-beginners-guide-to-using-can-in-your-projects-1239</t>
+        </is>
+      </c>
+      <c r="E76" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F76" s="4" t="inlineStr">
+        <is>
+          <t>#can, #arduino, #mcp2515</t>
+        </is>
+      </c>
+      <c r="G76" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H76" s="4" t="inlineStr"/>
+      <c r="I76" s="5" t="n">
+        <v>45816.69908564815</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="4" t="n">
+        <v>217</v>
+      </c>
+      <c r="B77" s="4" t="inlineStr">
+        <is>
+          <t>MVC in 10 Minutes: How Models, Views &amp; Controllers Actually Work (With Visual Diagrams)</t>
+        </is>
+      </c>
+      <c r="C77" s="4" t="inlineStr">
+        <is>
+          <t>Alex Aslam</t>
+        </is>
+      </c>
+      <c r="D77" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/alex_aslam/mvc-in-10-minutes-how-models-views-controllers-actually-work-with-visual-diagrams-ehi</t>
+        </is>
+      </c>
+      <c r="E77" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F77" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #programming, #javascript, #beginners</t>
+        </is>
+      </c>
+      <c r="G77" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="4" t="inlineStr"/>
+      <c r="I77" s="5" t="n">
+        <v>45816.84366898148</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="4" t="n">
+        <v>218</v>
+      </c>
+      <c r="B78" s="4" t="inlineStr">
+        <is>
+          <t>How to make splash screen with progress tracking in Angular?</t>
+        </is>
+      </c>
+      <c r="C78" s="4" t="inlineStr">
+        <is>
+          <t>Arek</t>
+        </is>
+      </c>
+      <c r="D78" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/theseith/how-to-make-splash-screen-with-progress-tracking-in-angular-49id</t>
+        </is>
+      </c>
+      <c r="E78" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F78" s="4" t="inlineStr">
+        <is>
+          <t>#angular, #webdev, #ux, #frontend</t>
+        </is>
+      </c>
+      <c r="G78" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="4" t="inlineStr"/>
+      <c r="I78" s="5" t="n">
+        <v>45816.84604166666</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="4" t="n">
+        <v>219</v>
+      </c>
+      <c r="B79" s="4" t="inlineStr">
+        <is>
+          <t>Understand Code Like an Editor: Intro to Tree-sitter</t>
+        </is>
+      </c>
+      <c r="C79" s="4" t="inlineStr">
+        <is>
+          <t>Rijul Rajesh</t>
+        </is>
+      </c>
+      <c r="D79" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/rijultp/understand-code-like-an-editor-intro-to-tree-sitter-50be</t>
+        </is>
+      </c>
+      <c r="E79" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F79" s="4" t="inlineStr">
+        <is>
+          <t>#c, #treesitter, #lint</t>
+        </is>
+      </c>
+      <c r="G79" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H79" s="4" t="inlineStr"/>
+      <c r="I79" s="5" t="n">
+        <v>45816.77997685185</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="4" t="n">
+        <v>220</v>
+      </c>
+      <c r="B80" s="4" t="inlineStr">
+        <is>
+          <t>Mail-Guide-AI: AI-Powered Email Management with Postmark Integration</t>
+        </is>
+      </c>
+      <c r="C80" s="4" t="inlineStr">
+        <is>
+          <t>Collins Dada</t>
+        </is>
+      </c>
+      <c r="D80" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/contractorx/mail-guide-ai-ai-powered-email-management-with-postmark-integration-5dof</t>
+        </is>
+      </c>
+      <c r="E80" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F80" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G80" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" s="4" t="inlineStr"/>
+      <c r="I80" s="5" t="n">
+        <v>45816.82424768519</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="4" t="n">
+        <v>221</v>
+      </c>
+      <c r="B81" s="4" t="inlineStr">
+        <is>
+          <t>Building an AI Voice Assistant in 1 Minute (Command Line)</t>
+        </is>
+      </c>
+      <c r="C81" s="4" t="inlineStr">
+        <is>
+          <t>Zuluana</t>
+        </is>
+      </c>
+      <c r="D81" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/zuluana/building-an-ai-voice-assistant-in-1-minute-command-line-n4i</t>
+        </is>
+      </c>
+      <c r="E81" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F81" s="4" t="inlineStr">
+        <is>
+          <t>#openai, #cli, #ai, #webdev</t>
+        </is>
+      </c>
+      <c r="G81" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" s="4" t="inlineStr"/>
+      <c r="I81" s="5" t="n">
+        <v>45816.71092592592</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="4" t="n">
+        <v>222</v>
+      </c>
+      <c r="B82" s="4" t="inlineStr">
+        <is>
+          <t>I Got Tired of Wrestling with YAML, So I Built a DevOps Helper in Rust 🚀</t>
+        </is>
+      </c>
+      <c r="C82" s="4" t="inlineStr">
+        <is>
+          <t>Alex Holmberg</t>
+        </is>
+      </c>
+      <c r="D82" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/alexthh_93/i-got-tired-of-wrestling-with-yaml-so-i-built-a-devops-helper-in-rust-15f3</t>
+        </is>
+      </c>
+      <c r="E82" s="5" t="n">
+        <v>45816.75223379629</v>
+      </c>
+      <c r="F82" s="4" t="inlineStr">
+        <is>
+          <t>#devops, #rust, #programming, #ai</t>
+        </is>
+      </c>
+      <c r="G82" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" s="4" t="inlineStr"/>
+      <c r="I82" s="5" t="n">
+        <v>45816.81688657407</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H30"/>
+  <autoFilter ref="A1:I82"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: atualização completa do scraper e geração avançada de relatórios
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_posts_devto.xlsx
+++ b/relatorios/relatorio_posts_devto.xlsx
@@ -11,9 +11,11 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gráfico Autores" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gráfico Reações" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gráfico Tags" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Gráfico Distribuição" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Wordcloud Tags" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$I$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$I$130</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -233,6 +235,66 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="9525000" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="5715000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11430000" cy="5715000"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -542,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -552,9 +614,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="5" customWidth="1" min="1" max="1"/>
-    <col width="118" customWidth="1" min="2" max="2"/>
+    <col width="250" customWidth="1" min="2" max="2"/>
     <col width="38" customWidth="1" min="3" max="3"/>
-    <col width="134" customWidth="1" min="4" max="4"/>
+    <col width="145" customWidth="1" min="4" max="4"/>
     <col width="21" customWidth="1" min="5" max="5"/>
     <col width="76" customWidth="1" min="6" max="6"/>
     <col width="9" customWidth="1" min="7" max="7"/>
@@ -3476,8 +3538,1690 @@
         <v>45816.81688657407</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" s="4" t="n">
+        <v>232</v>
+      </c>
+      <c r="B83" s="4" t="inlineStr">
+        <is>
+          <t>Loading Animation - Glow Pulse</t>
+        </is>
+      </c>
+      <c r="C83" s="4" t="inlineStr">
+        <is>
+          <t>Knight Witch</t>
+        </is>
+      </c>
+      <c r="D83" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/defcondelta88/loading-animation-glow-pulse-838</t>
+        </is>
+      </c>
+      <c r="E83" s="5" t="n">
+        <v>45816.76761574074</v>
+      </c>
+      <c r="F83" s="4" t="inlineStr">
+        <is>
+          <t>#codepen</t>
+        </is>
+      </c>
+      <c r="G83" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" s="4" t="inlineStr"/>
+      <c r="I83" s="5" t="n">
+        <v>45816.88091435185</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="4" t="n">
+        <v>245</v>
+      </c>
+      <c r="B84" s="4" t="inlineStr">
+        <is>
+          <t>Creating an animated website Using GSAP with Next.js and Tailwind CSS</t>
+        </is>
+      </c>
+      <c r="C84" s="4" t="inlineStr">
+        <is>
+          <t>Unnati Srivastava</t>
+        </is>
+      </c>
+      <c r="D84" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/unnati_srivastava_0430094/creating-an-animated-website-using-gsap-with-nextjs-and-tailwind-css-55ab</t>
+        </is>
+      </c>
+      <c r="E84" s="5" t="n">
+        <v>45816.76761574074</v>
+      </c>
+      <c r="F84" s="4" t="inlineStr">
+        <is>
+          <t>#gsap, #webdev, #nextjs, #tailwindcss</t>
+        </is>
+      </c>
+      <c r="G84" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" s="4" t="inlineStr"/>
+      <c r="I84" s="5" t="n">
+        <v>45816.8400462963</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="4" t="n">
+        <v>246</v>
+      </c>
+      <c r="B85" s="4" t="inlineStr">
+        <is>
+          <t>Track your expenses with email inbound!</t>
+        </is>
+      </c>
+      <c r="C85" s="4" t="inlineStr">
+        <is>
+          <t>Arthur Renard</t>
+        </is>
+      </c>
+      <c r="D85" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/arthur_renard_db96495494e/track-your-expenses-with-email-inbound-506g</t>
+        </is>
+      </c>
+      <c r="E85" s="5" t="n">
+        <v>45816.76761574074</v>
+      </c>
+      <c r="F85" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G85" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="4" t="inlineStr"/>
+      <c r="I85" s="5" t="n">
+        <v>45816.84127314815</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="4" t="n">
+        <v>247</v>
+      </c>
+      <c r="B86" s="4" t="inlineStr">
+        <is>
+          <t>Taming the Noise: How to Fix Garbage-in/Garbage-out AI Retrieval</t>
+        </is>
+      </c>
+      <c r="C86" s="4" t="inlineStr">
+        <is>
+          <t>Alex Aslam</t>
+        </is>
+      </c>
+      <c r="D86" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/alex_aslam/taming-the-noise-how-to-fix-garbage-ingarbage-out-ai-retrieval-1i6d</t>
+        </is>
+      </c>
+      <c r="E86" s="5" t="n">
+        <v>45816.76761574074</v>
+      </c>
+      <c r="F86" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #programming, #ai, #machinelearning</t>
+        </is>
+      </c>
+      <c r="G86" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" s="4" t="inlineStr"/>
+      <c r="I86" s="5" t="n">
+        <v>45816.83846064815</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="4" t="n">
+        <v>306</v>
+      </c>
+      <c r="B87" s="4" t="inlineStr">
+        <is>
+          <t>Understanding Domain Authority: What It Is and How to Achieve a High Score</t>
+        </is>
+      </c>
+      <c r="C87" s="4" t="inlineStr">
+        <is>
+          <t>Emeruche Ikenna</t>
+        </is>
+      </c>
+      <c r="D87" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/cole_ruche/understanding-domain-authority-what-it-is-and-how-to-achieve-a-high-score-2c5g</t>
+        </is>
+      </c>
+      <c r="E87" s="5" t="n">
+        <v>45816.7875</v>
+      </c>
+      <c r="F87" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G87" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="4" t="inlineStr"/>
+      <c r="I87" s="5" t="n">
+        <v>45816.90708333333</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="4" t="n">
+        <v>307</v>
+      </c>
+      <c r="B88" s="4" t="inlineStr">
+        <is>
+          <t>Coping With Receiving Comments on Your Pull Requests</t>
+        </is>
+      </c>
+      <c r="C88" s="4" t="inlineStr">
+        <is>
+          <t>Carlos Almonte</t>
+        </is>
+      </c>
+      <c r="D88" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/carlosrambles/coping-with-receiving-comments-on-your-pull-requests-4fb8</t>
+        </is>
+      </c>
+      <c r="E88" s="5" t="n">
+        <v>45816.7875</v>
+      </c>
+      <c r="F88" s="4" t="inlineStr">
+        <is>
+          <t>#react, #webdev, #programming, #javascript</t>
+        </is>
+      </c>
+      <c r="G88" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" s="4" t="inlineStr"/>
+      <c r="I88" s="5" t="n">
+        <v>45816.90733796296</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="4" t="n">
+        <v>309</v>
+      </c>
+      <c r="B89" s="4" t="inlineStr">
+        <is>
+          <t>ASP.NET 8 - Cookie Authentication</t>
+        </is>
+      </c>
+      <c r="C89" s="4" t="inlineStr">
+        <is>
+          <t>Vinícius Estevam</t>
+        </is>
+      </c>
+      <c r="D89" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/vinicius_estevam/aspnet-8-cookie-authentication-2o4j</t>
+        </is>
+      </c>
+      <c r="E89" s="5" t="n">
+        <v>45816.7875</v>
+      </c>
+      <c r="F89" s="4" t="inlineStr">
+        <is>
+          <t>#dotnetcore, #cookie, #csharp, #webdev</t>
+        </is>
+      </c>
+      <c r="G89" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" s="4" t="inlineStr"/>
+      <c r="I89" s="5" t="n">
+        <v>45816.89868055555</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="4" t="n">
+        <v>310</v>
+      </c>
+      <c r="B90" s="4" t="inlineStr">
+        <is>
+          <t>Introducing SnarkyType: The Snarkier way to type fast</t>
+        </is>
+      </c>
+      <c r="C90" s="4" t="inlineStr">
+        <is>
+          <t>Andrew McSillyone</t>
+        </is>
+      </c>
+      <c r="D90" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/codemonster240/introducing-snarkytype-the-snarkier-way-to-type-fast-h5l</t>
+        </is>
+      </c>
+      <c r="E90" s="5" t="n">
+        <v>45816.7875</v>
+      </c>
+      <c r="F90" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #productivity, #github</t>
+        </is>
+      </c>
+      <c r="G90" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="4" t="inlineStr"/>
+      <c r="I90" s="5" t="n">
+        <v>45816.89332175926</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="4" t="n">
+        <v>326</v>
+      </c>
+      <c r="B91" s="4" t="inlineStr">
+        <is>
+          <t>My ReadLater App Powered by Postmark</t>
+        </is>
+      </c>
+      <c r="C91" s="4" t="inlineStr">
+        <is>
+          <t>Bridget Amana</t>
+        </is>
+      </c>
+      <c r="D91" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/bridget_amana/my-readlater-app-powered-by-postmark-37d</t>
+        </is>
+      </c>
+      <c r="E91" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F91" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G91" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H91" s="4" t="inlineStr"/>
+      <c r="I91" s="5" t="n">
+        <v>45817.03472222222</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="4" t="n">
+        <v>327</v>
+      </c>
+      <c r="B92" s="4" t="inlineStr">
+        <is>
+          <t>🎯 AI Resume Ranking System</t>
+        </is>
+      </c>
+      <c r="C92" s="4" t="inlineStr">
+        <is>
+          <t>Vivek V.</t>
+        </is>
+      </c>
+      <c r="D92" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/aws-builders/ai-resume-ranking-system-2cok</t>
+        </is>
+      </c>
+      <c r="E92" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F92" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G92" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H92" s="4" t="inlineStr"/>
+      <c r="I92" s="5" t="n">
+        <v>45817.04224537037</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="4" t="n">
+        <v>328</v>
+      </c>
+      <c r="B93" s="4" t="inlineStr">
+        <is>
+          <t>SupportAddress — An email-first support platform</t>
+        </is>
+      </c>
+      <c r="C93" s="4" t="inlineStr">
+        <is>
+          <t>arnu515</t>
+        </is>
+      </c>
+      <c r="D93" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/arnu515/supportaddress-an-email-first-support-platform-1lo5</t>
+        </is>
+      </c>
+      <c r="E93" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F93" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G93" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" s="4" t="inlineStr"/>
+      <c r="I93" s="5" t="n">
+        <v>45817.00288194444</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="4" t="n">
+        <v>330</v>
+      </c>
+      <c r="B94" s="4" t="inlineStr">
+        <is>
+          <t>Hot Old Algorithms Looking for Features Near You!</t>
+        </is>
+      </c>
+      <c r="C94" s="4" t="inlineStr">
+        <is>
+          <t>Sarah Matta</t>
+        </is>
+      </c>
+      <c r="D94" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/sarahmatta/hot-old-algorithms-looking-for-features-near-you-1g8a</t>
+        </is>
+      </c>
+      <c r="E94" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F94" s="4" t="inlineStr">
+        <is>
+          <t>#algorithms, #programming, #machinelearning, #datastructures</t>
+        </is>
+      </c>
+      <c r="G94" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="4" t="inlineStr"/>
+      <c r="I94" s="5" t="n">
+        <v>45817.0646412037</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="4" t="n">
+        <v>331</v>
+      </c>
+      <c r="B95" s="4" t="inlineStr">
+        <is>
+          <t>Rawkode's Hands-on Intro to Fermyon Wasm Functions</t>
+        </is>
+      </c>
+      <c r="C95" s="4" t="inlineStr">
+        <is>
+          <t>Jasmine Mae</t>
+        </is>
+      </c>
+      <c r="D95" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/fermyon/rawkodes-hands-on-intro-to-fermyon-wasm-functions-1dca</t>
+        </is>
+      </c>
+      <c r="E95" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F95" s="4" t="inlineStr">
+        <is>
+          <t>#webassembly, #webdev, #learning, #programming</t>
+        </is>
+      </c>
+      <c r="G95" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" s="4" t="inlineStr"/>
+      <c r="I95" s="5" t="n">
+        <v>45817.04770833333</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="4" t="n">
+        <v>332</v>
+      </c>
+      <c r="B96" s="4" t="inlineStr">
+        <is>
+          <t>🎙️ Email-to-Podcast RSS Feed Generator using Node.js, OpenAI, ElevenLabs &amp; Postmark</t>
+        </is>
+      </c>
+      <c r="C96" s="4" t="inlineStr">
+        <is>
+          <t>Tom Canfarotta</t>
+        </is>
+      </c>
+      <c r="D96" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/tom_canfarotta_775a68254f/email-to-podcast-rss-feed-generator-using-nodejs-openai-elevenlabs-postmark-67l</t>
+        </is>
+      </c>
+      <c r="E96" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F96" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #devchallenge, #postmarkchallenge, #ai</t>
+        </is>
+      </c>
+      <c r="G96" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" s="4" t="inlineStr"/>
+      <c r="I96" s="5" t="n">
+        <v>45817.04761574074</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="4" t="n">
+        <v>333</v>
+      </c>
+      <c r="B97" s="4" t="inlineStr">
+        <is>
+          <t>Yazılımcılar için 5 Pratik İpucu</t>
+        </is>
+      </c>
+      <c r="C97" s="4" t="inlineStr">
+        <is>
+          <t>Yunus Emre Mert</t>
+        </is>
+      </c>
+      <c r="D97" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/yunus_emremert_1756b71d3/yazilimcilar-icin-5-pratik-ipucu-h96</t>
+        </is>
+      </c>
+      <c r="E97" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F97" s="4" t="inlineStr">
+        <is>
+          <t>#kodlama, #gelistirme, #verimlilik</t>
+        </is>
+      </c>
+      <c r="G97" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" s="4" t="inlineStr"/>
+      <c r="I97" s="5" t="n">
+        <v>45817.04739583333</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="4" t="n">
+        <v>334</v>
+      </c>
+      <c r="B98" s="4" t="inlineStr">
+        <is>
+          <t>A quick way to get started with Graphite</t>
+        </is>
+      </c>
+      <c r="C98" s="4" t="inlineStr">
+        <is>
+          <t>Brittney Kernan</t>
+        </is>
+      </c>
+      <c r="D98" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/brittneykernan/a-quick-way-to-get-started-with-graphite-5bb2</t>
+        </is>
+      </c>
+      <c r="E98" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F98" s="4" t="inlineStr">
+        <is>
+          <t>#graphite, #git, #webdev</t>
+        </is>
+      </c>
+      <c r="G98" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" s="4" t="inlineStr"/>
+      <c r="I98" s="5" t="n">
+        <v>45817.04746527778</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="4" t="n">
+        <v>335</v>
+      </c>
+      <c r="B99" s="4" t="inlineStr">
+        <is>
+          <t>I Built a Python Hangman Game and Pushed My First Project to GitHub</t>
+        </is>
+      </c>
+      <c r="C99" s="4" t="inlineStr">
+        <is>
+          <t>Rohan Nilatkar</t>
+        </is>
+      </c>
+      <c r="D99" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/iixpreyliet/i-built-a-python-hangman-game-and-pushed-my-first-project-to-github-389d</t>
+        </is>
+      </c>
+      <c r="E99" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F99" s="4" t="inlineStr">
+        <is>
+          <t>#python, #github, #beginners, #100daysofcode</t>
+        </is>
+      </c>
+      <c r="G99" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="4" t="inlineStr"/>
+      <c r="I99" s="5" t="n">
+        <v>45817.04702546296</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="4" t="n">
+        <v>336</v>
+      </c>
+      <c r="B100" s="4" t="inlineStr">
+        <is>
+          <t>EPB: Turn Emails into Code - AI-Powered Pull Requests from Your Inbox</t>
+        </is>
+      </c>
+      <c r="C100" s="4" t="inlineStr">
+        <is>
+          <t>B G Adam</t>
+        </is>
+      </c>
+      <c r="D100" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/async_dime/epb-turn-emails-into-code-ai-powered-pull-requests-from-your-inbox-33pg</t>
+        </is>
+      </c>
+      <c r="E100" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F100" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G100" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" s="4" t="inlineStr"/>
+      <c r="I100" s="5" t="n">
+        <v>45817.03505787037</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="4" t="n">
+        <v>337</v>
+      </c>
+      <c r="B101" s="4" t="inlineStr">
+        <is>
+          <t>Deep Dive into WaitGroup: Mastering Concurrent Task Orchestration in Go</t>
+        </is>
+      </c>
+      <c r="C101" s="4" t="inlineStr">
+        <is>
+          <t>Jones Charles</t>
+        </is>
+      </c>
+      <c r="D101" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jones_charles_ad50858dbc0/deep-dive-into-waitgroup-mastering-concurrent-task-orchestration-in-go-ao</t>
+        </is>
+      </c>
+      <c r="E101" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F101" s="4" t="inlineStr">
+        <is>
+          <t>#go, #programming, #tutorial, #beginners</t>
+        </is>
+      </c>
+      <c r="G101" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" s="4" t="inlineStr"/>
+      <c r="I101" s="5" t="n">
+        <v>45817.03561342593</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="4" t="n">
+        <v>338</v>
+      </c>
+      <c r="B102" s="4" t="inlineStr">
+        <is>
+          <t>Mastering the Pages Editor in Sitecore XM Cloud: Managing Page Content and Datasources</t>
+        </is>
+      </c>
+      <c r="C102" s="4" t="inlineStr">
+        <is>
+          <t>Sebastián Aliaga</t>
+        </is>
+      </c>
+      <c r="D102" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/sebasab/mastering-the-pages-editor-in-sitecore-xm-cloud-managing-page-content-and-datasources-5e33</t>
+        </is>
+      </c>
+      <c r="E102" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F102" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G102" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="4" t="inlineStr"/>
+      <c r="I102" s="5" t="n">
+        <v>45817.03885416667</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="4" t="n">
+        <v>340</v>
+      </c>
+      <c r="B103" s="4" t="inlineStr">
+        <is>
+          <t>About Likes</t>
+        </is>
+      </c>
+      <c r="C103" s="4" t="inlineStr">
+        <is>
+          <t>Andrey S Kalmatskiy</t>
+        </is>
+      </c>
+      <c r="D103" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/karol11/about-likes-2lpg</t>
+        </is>
+      </c>
+      <c r="E103" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F103" s="4" t="inlineStr">
+        <is>
+          <t>#ui, #web, #socialmedia</t>
+        </is>
+      </c>
+      <c r="G103" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" s="4" t="inlineStr"/>
+      <c r="I103" s="5" t="n">
+        <v>45817.04540509259</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="4" t="n">
+        <v>341</v>
+      </c>
+      <c r="B104" s="4" t="inlineStr">
+        <is>
+          <t>Postmark Challenge: Publish to Dev.to Straight from Your Inbox 📖</t>
+        </is>
+      </c>
+      <c r="C104" s="4" t="inlineStr">
+        <is>
+          <t>Raziel Rodrigues</t>
+        </is>
+      </c>
+      <c r="D104" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/razielrodrigues/postmark-challenge-publish-to-devto-straight-from-your-inbox-e16</t>
+        </is>
+      </c>
+      <c r="E104" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F104" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G104" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H104" s="4" t="inlineStr"/>
+      <c r="I104" s="5" t="n">
+        <v>45816.9455787037</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="4" t="n">
+        <v>343</v>
+      </c>
+      <c r="B105" s="4" t="inlineStr">
+        <is>
+          <t>Making Postr: Email-First App with Postmark's Inbound Parsing</t>
+        </is>
+      </c>
+      <c r="C105" s="4" t="inlineStr">
+        <is>
+          <t>Ansell Maximilian</t>
+        </is>
+      </c>
+      <c r="D105" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ansellmaximilian/making-postr-email-first-app-with-postmarks-inbound-parsing-3m9p</t>
+        </is>
+      </c>
+      <c r="E105" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F105" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G105" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H105" s="4" t="inlineStr"/>
+      <c r="I105" s="5" t="n">
+        <v>45817.06528935185</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="4" t="n">
+        <v>345</v>
+      </c>
+      <c r="B106" s="4" t="inlineStr">
+        <is>
+          <t>Deno vs Bun vs Node.js: The Ultimate Runtime Showdown</t>
+        </is>
+      </c>
+      <c r="C106" s="4" t="inlineStr">
+        <is>
+          <t>bilel salem</t>
+        </is>
+      </c>
+      <c r="D106" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/bilelsalemdev/deno-vs-bun-vs-nodejs-the-ultimate-runtime-showdown-4gn7</t>
+        </is>
+      </c>
+      <c r="E106" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F106" s="4" t="inlineStr">
+        <is>
+          <t>#node, #deno, #bunjs, #programming</t>
+        </is>
+      </c>
+      <c r="G106" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" s="4" t="inlineStr"/>
+      <c r="I106" s="5" t="n">
+        <v>45816.88510416666</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="4" t="n">
+        <v>346</v>
+      </c>
+      <c r="B107" s="4" t="inlineStr">
+        <is>
+          <t>How Can You Reverse Signs of Cell Values in Excel?</t>
+        </is>
+      </c>
+      <c r="C107" s="4" t="inlineStr">
+        <is>
+          <t>Vigneshwaran Vijayakumar</t>
+        </is>
+      </c>
+      <c r="D107" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/excel24x7/how-can-you-reverse-signs-of-cell-values-in-excel-2i36</t>
+        </is>
+      </c>
+      <c r="E107" s="5" t="n">
+        <v>45816.94680555556</v>
+      </c>
+      <c r="F107" s="4" t="inlineStr">
+        <is>
+          <t>#office, #excel, #tips, #beginners</t>
+        </is>
+      </c>
+      <c r="G107" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" s="4" t="inlineStr"/>
+      <c r="I107" s="5" t="n">
+        <v>45817.05416666667</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="4" t="n">
+        <v>366</v>
+      </c>
+      <c r="B108" s="4" t="inlineStr">
+        <is>
+          <t>Introducing Lily - a front end engineering agent you work with through email</t>
+        </is>
+      </c>
+      <c r="C108" s="4" t="inlineStr">
+        <is>
+          <t>Aaron Lebel</t>
+        </is>
+      </c>
+      <c r="D108" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/aaronlebel/introducing-lily-a-front-end-engineering-agent-you-work-with-through-email-9gg</t>
+        </is>
+      </c>
+      <c r="E108" s="5" t="n">
+        <v>45816.95320601852</v>
+      </c>
+      <c r="F108" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G108" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H108" s="4" t="inlineStr"/>
+      <c r="I108" s="5" t="n">
+        <v>45817.03240740741</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="4" t="n">
+        <v>368</v>
+      </c>
+      <c r="B109" s="4" t="inlineStr">
+        <is>
+          <t>HealthSync Mail - Medical Appointment Coordination</t>
+        </is>
+      </c>
+      <c r="C109" s="4" t="inlineStr">
+        <is>
+          <t>Arion Dev.ed</t>
+        </is>
+      </c>
+      <c r="D109" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ariondev/healthsync-mail-medical-appointment-coordination-598c</t>
+        </is>
+      </c>
+      <c r="E109" s="5" t="n">
+        <v>45816.95320601852</v>
+      </c>
+      <c r="F109" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G109" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" s="4" t="inlineStr"/>
+      <c r="I109" s="5" t="n">
+        <v>45817.06805555556</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="4" t="n">
+        <v>402</v>
+      </c>
+      <c r="B110" s="4" t="inlineStr">
+        <is>
+          <t>🌍 Beginner-Friendly Guide to Solving "K-th Smallest in Lexicographical Order" LeetCode 440 (C++ | JavaScript | Python)</t>
+        </is>
+      </c>
+      <c r="C110" s="4" t="inlineStr">
+        <is>
+          <t>Om Shree</t>
+        </is>
+      </c>
+      <c r="D110" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/om_shree_0709/beginner-friendly-guide-to-solving-k-th-smallest-in-lexicographical-order-leetcode-440-c--2il1</t>
+        </is>
+      </c>
+      <c r="E110" s="5" t="n">
+        <v>45816.97362268518</v>
+      </c>
+      <c r="F110" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #javascript, #cpp, #python</t>
+        </is>
+      </c>
+      <c r="G110" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H110" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I110" s="5" t="n">
+        <v>45817.09195601852</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="4" t="n">
+        <v>406</v>
+      </c>
+      <c r="B111" s="4" t="inlineStr">
+        <is>
+          <t>Applying matching algorithms to real allocation problems. Part 2</t>
+        </is>
+      </c>
+      <c r="C111" s="4" t="inlineStr">
+        <is>
+          <t>Deniss Sudak</t>
+        </is>
+      </c>
+      <c r="D111" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/denissudak/applying-matching-algorithms-to-real-allocation-problems-part-2-3ami</t>
+        </is>
+      </c>
+      <c r="E111" s="5" t="n">
+        <v>45816.97362268518</v>
+      </c>
+      <c r="F111" s="4" t="inlineStr">
+        <is>
+          <t>#graphtheory, #algorithms, #maximumflow, #combinatorial</t>
+        </is>
+      </c>
+      <c r="G111" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="4" t="inlineStr"/>
+      <c r="I111" s="5" t="n">
+        <v>45817.07549768518</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="4" t="n">
+        <v>407</v>
+      </c>
+      <c r="B112" s="4" t="inlineStr">
+        <is>
+          <t>Top 5 Mistakes I Made as a Beginner Web Developer</t>
+        </is>
+      </c>
+      <c r="C112" s="4" t="inlineStr">
+        <is>
+          <t>Vijay Kumar</t>
+        </is>
+      </c>
+      <c r="D112" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/vjygour/top-5-mistakes-i-made-as-a-beginner-web-developer-4k82</t>
+        </is>
+      </c>
+      <c r="E112" s="5" t="n">
+        <v>45816.97362268518</v>
+      </c>
+      <c r="F112" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #javascript, #programming, #beginners</t>
+        </is>
+      </c>
+      <c r="G112" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H112" s="4" t="inlineStr"/>
+      <c r="I112" s="5" t="n">
+        <v>45817.07716435185</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="4" t="n">
+        <v>470</v>
+      </c>
+      <c r="B113" s="4" t="inlineStr">
+        <is>
+          <t>Automating Git Sign-offs Per Project: A Complete Guide</t>
+        </is>
+      </c>
+      <c r="C113" s="4" t="inlineStr">
+        <is>
+          <t>GBTI Network</t>
+        </is>
+      </c>
+      <c r="D113" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/gbti-network/automating-git-sign-offs-per-project-a-complete-guide-mjp</t>
+        </is>
+      </c>
+      <c r="E113" s="5" t="n">
+        <v>45816.97894675926</v>
+      </c>
+      <c r="F113" s="4" t="inlineStr">
+        <is>
+          <t>#git, #devops, #tutorial, #automation</t>
+        </is>
+      </c>
+      <c r="G113" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H113" s="4" t="inlineStr"/>
+      <c r="I113" s="5" t="n">
+        <v>45817.09994212963</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="4" t="n">
+        <v>580</v>
+      </c>
+      <c r="B114" s="4" t="inlineStr">
+        <is>
+          <t>10 Squircles Worth Checking Out</t>
+        </is>
+      </c>
+      <c r="C114" s="4" t="inlineStr">
+        <is>
+          <t>Sarah Matta</t>
+        </is>
+      </c>
+      <c r="D114" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/sarahmatta/10-squircles-worth-checking-out-5cji</t>
+        </is>
+      </c>
+      <c r="E114" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F114" s="4" t="inlineStr">
+        <is>
+          <t>#css, #frontend, #webdev, #html</t>
+        </is>
+      </c>
+      <c r="G114" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H114" s="4" t="inlineStr"/>
+      <c r="I114" s="5" t="n">
+        <v>45817.0940162037</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="4" t="n">
+        <v>581</v>
+      </c>
+      <c r="B115" s="4" t="inlineStr">
+        <is>
+          <t>My Submission for the Postmark Challenge: I Turned My Inbox Into a Powerful Task Manager</t>
+        </is>
+      </c>
+      <c r="C115" s="4" t="inlineStr">
+        <is>
+          <t>Luis Fernando Richter</t>
+        </is>
+      </c>
+      <c r="D115" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/lfrichter/my-submission-for-the-postmark-challenge-i-turned-my-inbox-into-a-powerful-task-manager-2odd</t>
+        </is>
+      </c>
+      <c r="E115" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F115" s="4" t="inlineStr">
+        <is>
+          <t>#productivity, #postmarkchallenge, #laravel, #webhooks</t>
+        </is>
+      </c>
+      <c r="G115" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" s="4" t="inlineStr"/>
+      <c r="I115" s="5" t="n">
+        <v>45817.11458333334</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="4" t="n">
+        <v>582</v>
+      </c>
+      <c r="B116" s="4" t="inlineStr">
+        <is>
+          <t>HarmonyOS Next Interface Design Practice: Deep implementation from abstract contract to polymorphic programming</t>
+        </is>
+      </c>
+      <c r="C116" s="4" t="inlineStr">
+        <is>
+          <t>SameX</t>
+        </is>
+      </c>
+      <c r="D116" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/xun_wang_6384a403f9817c2/harmonyos-next-interface-design-practice-deep-implementation-from-abstract-contract-to-polymorphic-10kh</t>
+        </is>
+      </c>
+      <c r="E116" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F116" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G116" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="4" t="inlineStr"/>
+      <c r="I116" s="5" t="n">
+        <v>45817.11796296296</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="4" t="n">
+        <v>584</v>
+      </c>
+      <c r="B117" s="4" t="inlineStr">
+        <is>
+          <t>A pivot back to Flutter</t>
+        </is>
+      </c>
+      <c r="C117" s="4" t="inlineStr">
+        <is>
+          <t>Dan Dahl</t>
+        </is>
+      </c>
+      <c r="D117" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/magipunk/a-pivot-back-to-flutter-lgb</t>
+        </is>
+      </c>
+      <c r="E117" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F117" s="4" t="inlineStr">
+        <is>
+          <t>#flutter, #gamedev</t>
+        </is>
+      </c>
+      <c r="G117" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" s="4" t="inlineStr"/>
+      <c r="I117" s="5" t="n">
+        <v>45817.09309027778</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="4" t="n">
+        <v>585</v>
+      </c>
+      <c r="B118" s="4" t="inlineStr">
+        <is>
+          <t>JavaScript this Explained — With Simple Examples</t>
+        </is>
+      </c>
+      <c r="C118" s="4" t="inlineStr">
+        <is>
+          <t>Manoj</t>
+        </is>
+      </c>
+      <c r="D118" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/manoj257/javascript-this-explained-with-simple-examples-1n21</t>
+        </is>
+      </c>
+      <c r="E118" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F118" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G118" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="4" t="inlineStr"/>
+      <c r="I118" s="5" t="n">
+        <v>45817.09846064815</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="4" t="n">
+        <v>586</v>
+      </c>
+      <c r="B119" s="4" t="inlineStr">
+        <is>
+          <t>⚠️ Upskill or Get Replaced: The Brutal Reality of Modern Software Jobs</t>
+        </is>
+      </c>
+      <c r="C119" s="4" t="inlineStr">
+        <is>
+          <t>Raj Aryan</t>
+        </is>
+      </c>
+      <c r="D119" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/er-raj-aryan/upskill-or-get-replaced-the-brutal-reality-of-modern-software-jobs-284m</t>
+        </is>
+      </c>
+      <c r="E119" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F119" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G119" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" s="4" t="inlineStr"/>
+      <c r="I119" s="5" t="n">
+        <v>45817.0983912037</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="4" t="n">
+        <v>587</v>
+      </c>
+      <c r="B120" s="4" t="inlineStr">
+        <is>
+          <t>FeedLoop : Email-Based Feedback System</t>
+        </is>
+      </c>
+      <c r="C120" s="4" t="inlineStr">
+        <is>
+          <t>Umar (Cynexium)</t>
+        </is>
+      </c>
+      <c r="D120" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/cynexium/feedloop-email-based-feedback-system-m5f</t>
+        </is>
+      </c>
+      <c r="E120" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F120" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G120" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" s="4" t="inlineStr"/>
+      <c r="I120" s="5" t="n">
+        <v>45817.10109953704</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="4" t="n">
+        <v>588</v>
+      </c>
+      <c r="B121" s="4" t="inlineStr">
+        <is>
+          <t>SQL vs NoSQL</t>
+        </is>
+      </c>
+      <c r="C121" s="4" t="inlineStr">
+        <is>
+          <t>Manoj</t>
+        </is>
+      </c>
+      <c r="D121" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/manoj257/sql-vs-nosql-4219</t>
+        </is>
+      </c>
+      <c r="E121" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F121" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G121" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" s="4" t="inlineStr"/>
+      <c r="I121" s="5" t="n">
+        <v>45817.09293981481</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="4" t="n">
+        <v>593</v>
+      </c>
+      <c r="B122" s="4" t="inlineStr">
+        <is>
+          <t>🚀 DixitCoder AI Control Panel Browser – Secure, Stylish, and Tor-Ready!</t>
+        </is>
+      </c>
+      <c r="C122" s="4" t="inlineStr">
+        <is>
+          <t>dixit patel</t>
+        </is>
+      </c>
+      <c r="D122" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/dixitcoder/dixitcoder-ai-control-panel-browser-secure-stylish-and-tor-ready-1ofc</t>
+        </is>
+      </c>
+      <c r="E122" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F122" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G122" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" s="4" t="inlineStr"/>
+      <c r="I122" s="5" t="n">
+        <v>45817.09506944445</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="4" t="n">
+        <v>594</v>
+      </c>
+      <c r="B123" s="4" t="inlineStr">
+        <is>
+          <t>Learn how to automate Git sign-offs at the project level using commit templates, aliases, and scripts, ensuring proper sign-offs without disrupting workflow. https://gbti.network/devops/frameworks/git/how-to-automatically-sign-off-git-commits/ #Git</t>
+        </is>
+      </c>
+      <c r="C123" s="4" t="inlineStr">
+        <is>
+          <t>GBTI Network</t>
+        </is>
+      </c>
+      <c r="D123" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/gbti/learn-how-to-automate-git-sign-offs-at-the-project-level-using-commit-templates-aliases-and-olm</t>
+        </is>
+      </c>
+      <c r="E123" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F123" s="4" t="inlineStr">
+        <is>
+          <t>#git, #github, #automation, #devops</t>
+        </is>
+      </c>
+      <c r="G123" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H123" s="4" t="inlineStr"/>
+      <c r="I123" s="5" t="n">
+        <v>45817.09445601852</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="4" t="n">
+        <v>595</v>
+      </c>
+      <c r="B124" s="4" t="inlineStr">
+        <is>
+          <t>Reimagining API Integration for AI: The Case for MCP Over HTTP</t>
+        </is>
+      </c>
+      <c r="C124" s="4" t="inlineStr">
+        <is>
+          <t>Venkata</t>
+        </is>
+      </c>
+      <c r="D124" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/nagarakesh4/reimagining-api-integration-for-ai-the-case-for-mcp-over-http-5gbk</t>
+        </is>
+      </c>
+      <c r="E124" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F124" s="4" t="inlineStr">
+        <is>
+          <t>#mcp, #modelcontextprotocol, #mcpvsapi</t>
+        </is>
+      </c>
+      <c r="G124" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H124" s="4" t="inlineStr"/>
+      <c r="I124" s="5" t="n">
+        <v>45817.12231481481</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="4" t="n">
+        <v>596</v>
+      </c>
+      <c r="B125" s="4" t="inlineStr">
+        <is>
+          <t>🧪 Understanding the ACID Properties in Databases</t>
+        </is>
+      </c>
+      <c r="C125" s="4" t="inlineStr">
+        <is>
+          <t>Sajidur Rahman Shajib</t>
+        </is>
+      </c>
+      <c r="D125" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/sajidurshajib/understanding-the-acid-properties-in-databases-m2i</t>
+        </is>
+      </c>
+      <c r="E125" s="5" t="n">
+        <v>45817.00027777778</v>
+      </c>
+      <c r="F125" s="4" t="inlineStr">
+        <is>
+          <t>#database, #acid, #webdev, #softwaredevelopment</t>
+        </is>
+      </c>
+      <c r="G125" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" s="4" t="inlineStr"/>
+      <c r="I125" s="5" t="n">
+        <v>45817.11847222222</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="4" t="n">
+        <v>657</v>
+      </c>
+      <c r="B126" s="4" t="inlineStr">
+        <is>
+          <t>How to Make SVGs Accessible: A Short Guide</t>
+        </is>
+      </c>
+      <c r="C126" s="4" t="inlineStr">
+        <is>
+          <t>Accessibly Speaking</t>
+        </is>
+      </c>
+      <c r="D126" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/accessibly_speaking/how-to-make-svgs-accessible-a-short-guide-1ope</t>
+        </is>
+      </c>
+      <c r="E126" s="5" t="n">
+        <v>45817.01290509259</v>
+      </c>
+      <c r="F126" s="4" t="inlineStr">
+        <is>
+          <t>#a11y, #webdev, #beginners, #developers</t>
+        </is>
+      </c>
+      <c r="G126" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H126" s="4" t="inlineStr"/>
+      <c r="I126" s="5" t="n">
+        <v>45817.12430555555</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="4" t="n">
+        <v>658</v>
+      </c>
+      <c r="B127" s="4" t="inlineStr">
+        <is>
+          <t>We created an application called **Identity Attestation via Hiring Emails**.</t>
+        </is>
+      </c>
+      <c r="C127" s="4" t="inlineStr">
+        <is>
+          <t>Felipe Segall Corrêa</t>
+        </is>
+      </c>
+      <c r="D127" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/fsegall/we-created-an-application-called-identity-attestation-via-hiring-emails-20nn</t>
+        </is>
+      </c>
+      <c r="E127" s="5" t="n">
+        <v>45817.01290509259</v>
+      </c>
+      <c r="F127" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G127" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" s="4" t="inlineStr"/>
+      <c r="I127" s="5" t="n">
+        <v>45817.12449074074</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="4" t="n">
+        <v>659</v>
+      </c>
+      <c r="B128" s="4" t="inlineStr">
+        <is>
+          <t>How to Filter a Collection Using Streams in Java?</t>
+        </is>
+      </c>
+      <c r="C128" s="4" t="inlineStr">
+        <is>
+          <t>Aditya Pratap Bhuyan</t>
+        </is>
+      </c>
+      <c r="D128" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/adityabhuyan/how-to-filter-a-collection-using-streams-in-java-13np</t>
+        </is>
+      </c>
+      <c r="E128" s="5" t="n">
+        <v>45817.01290509259</v>
+      </c>
+      <c r="F128" s="4" t="inlineStr">
+        <is>
+          <t>#java, #java8, #stream, #filter</t>
+        </is>
+      </c>
+      <c r="G128" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" s="4" t="inlineStr"/>
+      <c r="I128" s="5" t="n">
+        <v>45817.12472222222</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="4" t="n">
+        <v>660</v>
+      </c>
+      <c r="B129" s="4" t="inlineStr">
+        <is>
+          <t>Duolingo’s Shallow Learning Trap: Gamified Streaks, Harmful Habits</t>
+        </is>
+      </c>
+      <c r="C129" s="4" t="inlineStr">
+        <is>
+          <t>Christian</t>
+        </is>
+      </c>
+      <c r="D129" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/yaptech/duolingos-shallow-learning-trap-gamified-streaks-harmful-habits-4134</t>
+        </is>
+      </c>
+      <c r="E129" s="5" t="n">
+        <v>45817.01290509259</v>
+      </c>
+      <c r="F129" s="4" t="inlineStr">
+        <is>
+          <t>#learning, #founder, #edtech, #startup</t>
+        </is>
+      </c>
+      <c r="G129" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" s="4" t="inlineStr"/>
+      <c r="I129" s="5" t="n">
+        <v>45817.12484953704</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="4" t="n">
+        <v>662</v>
+      </c>
+      <c r="B130" s="4" t="inlineStr">
+        <is>
+          <t>Weak concepts can cost you</t>
+        </is>
+      </c>
+      <c r="C130" s="4" t="inlineStr">
+        <is>
+          <t>Derm</t>
+        </is>
+      </c>
+      <c r="D130" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/dermotholmes/weak-concepts-can-cost-you-5aih</t>
+        </is>
+      </c>
+      <c r="E130" s="5" t="n">
+        <v>45817.01290509259</v>
+      </c>
+      <c r="F130" s="4" t="inlineStr">
+        <is>
+          <t>#ai, #softwaredevelopment, #design, #concept</t>
+        </is>
+      </c>
+      <c r="G130" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" s="4" t="inlineStr"/>
+      <c r="I130" s="5" t="n">
+        <v>45817.09116898148</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I82"/>
+  <autoFilter ref="A1:I130"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3537,4 +5281,42 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Projeto Final - Com Dashboard e publicador no x
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_posts_devto.xlsx
+++ b/relatorios/relatorio_posts_devto.xlsx
@@ -15,7 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Wordcloud Tags" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$I$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Posts'!$A$1:$I$185</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:I185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -613,7 +613,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="5" customWidth="1" min="1" max="1"/>
+    <col width="6" customWidth="1" min="1" max="1"/>
     <col width="250" customWidth="1" min="2" max="2"/>
     <col width="38" customWidth="1" min="3" max="3"/>
     <col width="145" customWidth="1" min="4" max="4"/>
@@ -5220,8 +5220,1945 @@
         <v>45817.09116898148</v>
       </c>
     </row>
+    <row r="131">
+      <c r="A131" s="4" t="n">
+        <v>698</v>
+      </c>
+      <c r="B131" s="4" t="inlineStr">
+        <is>
+          <t>Meme Monday</t>
+        </is>
+      </c>
+      <c r="C131" s="4" t="inlineStr">
+        <is>
+          <t>Ben Halpern</t>
+        </is>
+      </c>
+      <c r="D131" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ben/meme-monday-g2o</t>
+        </is>
+      </c>
+      <c r="E131" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F131" s="4" t="inlineStr">
+        <is>
+          <t>#discuss, #watercooler, #jokes</t>
+        </is>
+      </c>
+      <c r="G131" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H131" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I131" s="5" t="n">
+        <v>45817.55724537037</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="4" t="n">
+        <v>700</v>
+      </c>
+      <c r="B132" s="4" t="inlineStr">
+        <is>
+          <t>PR Reminder: From Email Chaos to Slack Magic ⚡</t>
+        </is>
+      </c>
+      <c r="C132" s="4" t="inlineStr">
+        <is>
+          <t>Bartholomew Bassey</t>
+        </is>
+      </c>
+      <c r="D132" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/barth007/pr-reminder-from-email-chaos-to-slack-magic-2hf0</t>
+        </is>
+      </c>
+      <c r="E132" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F132" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G132" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="H132" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="I132" s="5" t="n">
+        <v>45817.24976851852</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="4" t="n">
+        <v>701</v>
+      </c>
+      <c r="B133" s="4" t="inlineStr">
+        <is>
+          <t>Understanding Local and Remote Model Context Protocols</t>
+        </is>
+      </c>
+      <c r="C133" s="4" t="inlineStr">
+        <is>
+          <t>𝚂𝚊𝚞𝚛𝚊𝚋𝚑 𝚁𝚊𝚒</t>
+        </is>
+      </c>
+      <c r="D133" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/apideck/understanding-local-and-remote-model-context-protocols-5b26</t>
+        </is>
+      </c>
+      <c r="E133" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F133" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #mcp, #ai, #webdev</t>
+        </is>
+      </c>
+      <c r="G133" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="H133" s="4" t="inlineStr"/>
+      <c r="I133" s="5" t="n">
+        <v>45817.3708449074</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="4" t="n">
+        <v>702</v>
+      </c>
+      <c r="B134" s="4" t="inlineStr">
+        <is>
+          <t>☁️ From On-Prem to AWS: Your Complete Migration Roadmap🚀</t>
+        </is>
+      </c>
+      <c r="C134" s="4" t="inlineStr">
+        <is>
+          <t>Sarvar Nadaf</t>
+        </is>
+      </c>
+      <c r="D134" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/aws-builders/from-on-prem-to-aws-your-complete-migration-roadmap-ah1</t>
+        </is>
+      </c>
+      <c r="E134" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F134" s="4" t="inlineStr">
+        <is>
+          <t>#aws, #programming, #devops, #beginners</t>
+        </is>
+      </c>
+      <c r="G134" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H134" s="4" t="inlineStr"/>
+      <c r="I134" s="5" t="n">
+        <v>45817.54234953703</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="4" t="n">
+        <v>703</v>
+      </c>
+      <c r="B135" s="4" t="inlineStr">
+        <is>
+          <t>Charts in CSS</t>
+        </is>
+      </c>
+      <c r="C135" s="4" t="inlineStr">
+        <is>
+          <t>Mads Stoumann</t>
+        </is>
+      </c>
+      <c r="D135" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/madsstoumann/charts-in-css-1di1</t>
+        </is>
+      </c>
+      <c r="E135" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F135" s="4" t="inlineStr">
+        <is>
+          <t>#showdev, #css, #tutorial, #webdev</t>
+        </is>
+      </c>
+      <c r="G135" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H135" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I135" s="5" t="n">
+        <v>45817.44695601852</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="4" t="n">
+        <v>704</v>
+      </c>
+      <c r="B136" s="4" t="inlineStr">
+        <is>
+          <t>🎯 How to Format Numbers &amp; Currencies in Bubble (Bubble.io Tutorial)</t>
+        </is>
+      </c>
+      <c r="C136" s="4" t="inlineStr">
+        <is>
+          <t>NJOKU SAMSON EBERE</t>
+        </is>
+      </c>
+      <c r="D136" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ebereplenty/how-to-format-numbers-currencies-in-bubble-bubbleio-tutorial-3hjl</t>
+        </is>
+      </c>
+      <c r="E136" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F136" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #programming, #beginners, #noco</t>
+        </is>
+      </c>
+      <c r="G136" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" s="4" t="inlineStr"/>
+      <c r="I136" s="5" t="n">
+        <v>45817.49902777778</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="4" t="n">
+        <v>705</v>
+      </c>
+      <c r="B137" s="4" t="inlineStr">
+        <is>
+          <t>Become a Docker Superstar - part 1</t>
+        </is>
+      </c>
+      <c r="C137" s="4" t="inlineStr">
+        <is>
+          <t>Ibrahim Bagalwa</t>
+        </is>
+      </c>
+      <c r="D137" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ibrahimbagalwa/become-a-docker-superstar-part-1-p54</t>
+        </is>
+      </c>
+      <c r="E137" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F137" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #devops, #docker, #cloudnative</t>
+        </is>
+      </c>
+      <c r="G137" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H137" s="4" t="inlineStr"/>
+      <c r="I137" s="5" t="n">
+        <v>45817.49804398148</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="4" t="n">
+        <v>706</v>
+      </c>
+      <c r="B138" s="4" t="inlineStr">
+        <is>
+          <t>What are your goals for the week? #130</t>
+        </is>
+      </c>
+      <c r="C138" s="4" t="inlineStr">
+        <is>
+          <t>Chris Jarvis</t>
+        </is>
+      </c>
+      <c r="D138" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jarvisscript/what-are-your-goals-for-the-week-130-3912</t>
+        </is>
+      </c>
+      <c r="E138" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F138" s="4" t="inlineStr">
+        <is>
+          <t>#discuss, #motivation, #productivity</t>
+        </is>
+      </c>
+      <c r="G138" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H138" s="4" t="inlineStr"/>
+      <c r="I138" s="5" t="n">
+        <v>45817.57256944444</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="4" t="n">
+        <v>707</v>
+      </c>
+      <c r="B139" s="4" t="inlineStr">
+        <is>
+          <t>Decoding the Answer: How Copilot Studio’s Gen AI Orchestration Handles Complex Policy Queries</t>
+        </is>
+      </c>
+      <c r="C139" s="4" t="inlineStr">
+        <is>
+          <t>Bala Madhusoodhanan</t>
+        </is>
+      </c>
+      <c r="D139" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/balagmadhu/decoding-the-answer-how-copilot-studios-gen-ai-orchestration-handles-complex-policy-queries-35cj</t>
+        </is>
+      </c>
+      <c r="E139" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F139" s="4" t="inlineStr">
+        <is>
+          <t>#powerplatform, #copilotstudio, #genai, #powerfuldevs</t>
+        </is>
+      </c>
+      <c r="G139" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H139" s="4" t="inlineStr"/>
+      <c r="I139" s="5" t="n">
+        <v>45817.29204861111</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="4" t="n">
+        <v>708</v>
+      </c>
+      <c r="B140" s="4" t="inlineStr">
+        <is>
+          <t>Shell/Python vs Go - practical notes form a reimplementation project</t>
+        </is>
+      </c>
+      <c r="C140" s="4" t="inlineStr">
+        <is>
+          <t>TaiKedz</t>
+        </is>
+      </c>
+      <c r="D140" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/taikedz/shell-scripting-vs-go-practical-notes-form-a-reimplementation-project-1b18</t>
+        </is>
+      </c>
+      <c r="E140" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F140" s="4" t="inlineStr">
+        <is>
+          <t>#go, #bash, #python, #comparison</t>
+        </is>
+      </c>
+      <c r="G140" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="4" t="inlineStr"/>
+      <c r="I140" s="5" t="n">
+        <v>45817.56932870371</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="4" t="n">
+        <v>709</v>
+      </c>
+      <c r="B141" s="4" t="inlineStr">
+        <is>
+          <t>Slapp.dev, ship apps without leaving your inbox</t>
+        </is>
+      </c>
+      <c r="C141" s="4" t="inlineStr">
+        <is>
+          <t>Joshua Omobola</t>
+        </is>
+      </c>
+      <c r="D141" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/koha/slappdev-ship-apps-without-leaving-your-inbox-ph1</t>
+        </is>
+      </c>
+      <c r="E141" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F141" s="4" t="inlineStr">
+        <is>
+          <t>#devchallenge, #postmarkchallenge, #webdev, #api</t>
+        </is>
+      </c>
+      <c r="G141" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="H141" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I141" s="5" t="n">
+        <v>45817.28321759259</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="4" t="n">
+        <v>710</v>
+      </c>
+      <c r="B142" s="4" t="inlineStr">
+        <is>
+          <t>Partage de données entre composants RiotJS avec Mitt (émetteur d'évènements)</t>
+        </is>
+      </c>
+      <c r="C142" s="4" t="inlineStr">
+        <is>
+          <t>Steeve</t>
+        </is>
+      </c>
+      <c r="D142" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/steeve/partage-de-donnees-entre-composants-riotjs-avec-mitt-emetteur-devenements-31di</t>
+        </is>
+      </c>
+      <c r="E142" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F142" s="4" t="inlineStr">
+        <is>
+          <t>#riotjs, #french, #frontend, #javascript</t>
+        </is>
+      </c>
+      <c r="G142" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" s="4" t="inlineStr"/>
+      <c r="I142" s="5" t="n">
+        <v>45817.5</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="4" t="n">
+        <v>711</v>
+      </c>
+      <c r="B143" s="4" t="inlineStr">
+        <is>
+          <t>Optimized Fonts in Nuxt</t>
+        </is>
+      </c>
+      <c r="C143" s="4" t="inlineStr">
+        <is>
+          <t>Jakub Andrzejewski</t>
+        </is>
+      </c>
+      <c r="D143" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jacobandrewsky/optimized-fonts-in-nuxt-2a1n</t>
+        </is>
+      </c>
+      <c r="E143" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F143" s="4" t="inlineStr">
+        <is>
+          <t>#performance, #nuxt, #vue, #typescript</t>
+        </is>
+      </c>
+      <c r="G143" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" s="4" t="inlineStr"/>
+      <c r="I143" s="5" t="n">
+        <v>45817.2812037037</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="4" t="n">
+        <v>712</v>
+      </c>
+      <c r="B144" s="4" t="inlineStr">
+        <is>
+          <t>The Rust Renaissance: Why OpenAI and the Tech World Are Shifting from Node.js for High-Performance Tools</t>
+        </is>
+      </c>
+      <c r="C144" s="4" t="inlineStr">
+        <is>
+          <t>Platypus</t>
+        </is>
+      </c>
+      <c r="D144" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/platypus98/the-rust-renaissance-why-openai-and-the-tech-world-are-shifting-from-nodejs-for-high-performance-5561</t>
+        </is>
+      </c>
+      <c r="E144" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F144" s="4" t="inlineStr">
+        <is>
+          <t>#openai, #node, #rust, #programming</t>
+        </is>
+      </c>
+      <c r="G144" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H144" s="4" t="inlineStr"/>
+      <c r="I144" s="5" t="n">
+        <v>45817.45871527777</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="4" t="n">
+        <v>713</v>
+      </c>
+      <c r="B145" s="4" t="inlineStr">
+        <is>
+          <t>How to Prevent Network Eavesdropping and Data Theft by Highly Skilled IT Professionals such as Jeremy Nevins</t>
+        </is>
+      </c>
+      <c r="C145" s="4" t="inlineStr">
+        <is>
+          <t>Jeremy Nevins</t>
+        </is>
+      </c>
+      <c r="D145" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jnevins1/how-to-prevent-network-eavesdropping-and-data-theft-by-highly-skilled-it-professionals-such-as-55cn</t>
+        </is>
+      </c>
+      <c r="E145" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F145" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G145" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="4" t="inlineStr"/>
+      <c r="I145" s="5" t="n">
+        <v>45817.56494212963</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="4" t="n">
+        <v>714</v>
+      </c>
+      <c r="B146" s="4" t="inlineStr">
+        <is>
+          <t>How to Deploy a Full Stack App to Koyeb Using Docker Compose and GitLab CI/CD</t>
+        </is>
+      </c>
+      <c r="C146" s="4" t="inlineStr">
+        <is>
+          <t>EphraimX</t>
+        </is>
+      </c>
+      <c r="D146" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ephraimx/how-to-deploy-a-full-stack-app-to-koyeb-using-docker-compose-and-gitlab-cicd-2mk3</t>
+        </is>
+      </c>
+      <c r="E146" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F146" s="4" t="inlineStr">
+        <is>
+          <t>#devops, #gitlab, #docker, #koyeb</t>
+        </is>
+      </c>
+      <c r="G146" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" s="4" t="inlineStr"/>
+      <c r="I146" s="5" t="n">
+        <v>45817.57094907408</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="4" t="n">
+        <v>715</v>
+      </c>
+      <c r="B147" s="4" t="inlineStr">
+        <is>
+          <t>The 5 Most Popular Ways APIs Communicate Today</t>
+        </is>
+      </c>
+      <c r="C147" s="4" t="inlineStr">
+        <is>
+          <t>Igor Vorobiov</t>
+        </is>
+      </c>
+      <c r="D147" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ivorobioff/the-5-most-popular-ways-apis-communicate-today-1koe</t>
+        </is>
+      </c>
+      <c r="E147" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F147" s="4" t="inlineStr">
+        <is>
+          <t>#api, #rest, #microservices, #software</t>
+        </is>
+      </c>
+      <c r="G147" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="4" t="inlineStr"/>
+      <c r="I147" s="5" t="n">
+        <v>45817.5721875</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="4" t="n">
+        <v>716</v>
+      </c>
+      <c r="B148" s="4" t="inlineStr">
+        <is>
+          <t>Deploy a Dockerized App to AWS EKS Using EC2</t>
+        </is>
+      </c>
+      <c r="C148" s="4" t="inlineStr">
+        <is>
+          <t>SNS-Srinivasu</t>
+        </is>
+      </c>
+      <c r="D148" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/sukuru_naga_sai_srinivasu/deploy-a-dockerized-app-to-aws-eks-using-ec2-1d5h</t>
+        </is>
+      </c>
+      <c r="E148" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F148" s="4" t="inlineStr">
+        <is>
+          <t>#aws, #kubernetes, #docker, #github</t>
+        </is>
+      </c>
+      <c r="G148" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" s="4" t="inlineStr"/>
+      <c r="I148" s="5" t="n">
+        <v>45817.56783564815</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="4" t="n">
+        <v>717</v>
+      </c>
+      <c r="B149" s="4" t="inlineStr">
+        <is>
+          <t>Answering the Interview Question: "How Do You Review Code as a Tech Lead?"</t>
+        </is>
+      </c>
+      <c r="C149" s="4" t="inlineStr">
+        <is>
+          <t>Kris Chou</t>
+        </is>
+      </c>
+      <c r="D149" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/kris_chou_5f6deb607e8cb75/answering-the-interview-question-how-do-you-review-code-as-a-tech-lead-2671</t>
+        </is>
+      </c>
+      <c r="E149" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F149" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #softwaredevelopment, #interview, #career</t>
+        </is>
+      </c>
+      <c r="G149" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="4" t="inlineStr"/>
+      <c r="I149" s="5" t="n">
+        <v>45817.57118055555</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="4" t="n">
+        <v>718</v>
+      </c>
+      <c r="B150" s="4" t="inlineStr">
+        <is>
+          <t>How to Effectively Preprocess and Scale Your Data</t>
+        </is>
+      </c>
+      <c r="C150" s="4" t="inlineStr">
+        <is>
+          <t>Aaryan</t>
+        </is>
+      </c>
+      <c r="D150" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/dev_aaryan_9799/how-to-effectively-preprocess-and-scale-your-data-f0d</t>
+        </is>
+      </c>
+      <c r="E150" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F150" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #ai, #machinelearning, #datascience</t>
+        </is>
+      </c>
+      <c r="G150" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" s="4" t="inlineStr"/>
+      <c r="I150" s="5" t="n">
+        <v>45817.57068287037</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="4" t="n">
+        <v>719</v>
+      </c>
+      <c r="B151" s="4" t="inlineStr">
+        <is>
+          <t>JUCE: Revolutionizing Cross-Platform C++ Development</t>
+        </is>
+      </c>
+      <c r="C151" s="4" t="inlineStr">
+        <is>
+          <t>GitHubOpenSource</t>
+        </is>
+      </c>
+      <c r="D151" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/githubopensource/juce-revolutionizing-cross-platform-c-development-33fk</t>
+        </is>
+      </c>
+      <c r="E151" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F151" s="4" t="inlineStr">
+        <is>
+          <t>#c, #crossplatform, #audio, #juce</t>
+        </is>
+      </c>
+      <c r="G151" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="4" t="inlineStr"/>
+      <c r="I151" s="5" t="n">
+        <v>45817.56216435185</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="4" t="n">
+        <v>720</v>
+      </c>
+      <c r="B152" s="4" t="inlineStr">
+        <is>
+          <t>Python Dictionary Methods All in One</t>
+        </is>
+      </c>
+      <c r="C152" s="4" t="inlineStr">
+        <is>
+          <t>Omor Faruk</t>
+        </is>
+      </c>
+      <c r="D152" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/theonlineaid/python-dictionary-methods-all-in-one-3n6o</t>
+        </is>
+      </c>
+      <c r="E152" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F152" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #ai, #tutorial, #python</t>
+        </is>
+      </c>
+      <c r="G152" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H152" s="4" t="inlineStr"/>
+      <c r="I152" s="5" t="n">
+        <v>45817.55371527778</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="4" t="n">
+        <v>721</v>
+      </c>
+      <c r="B153" s="4" t="inlineStr">
+        <is>
+          <t>Harmonyos Next Cangjie Language Development Practical Tutorial: Store Detail Page</t>
+        </is>
+      </c>
+      <c r="C153" s="4" t="inlineStr">
+        <is>
+          <t>wei chang</t>
+        </is>
+      </c>
+      <c r="D153" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/youlanjihua/harmonyos-next-cangjie-language-development-practical-tutorial-store-detail-page-24db</t>
+        </is>
+      </c>
+      <c r="E153" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F153" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G153" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H153" s="4" t="inlineStr"/>
+      <c r="I153" s="5" t="n">
+        <v>45817.55403935185</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="4" t="n">
+        <v>722</v>
+      </c>
+      <c r="B154" s="4" t="inlineStr">
+        <is>
+          <t>Architecting a Scalable Voice Cloning Platform on AWS: A Case Study</t>
+        </is>
+      </c>
+      <c r="C154" s="4" t="inlineStr">
+        <is>
+          <t>Todd Bernson</t>
+        </is>
+      </c>
+      <c r="D154" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/semperfitodd/architecting-a-scalable-voice-cloning-platform-on-aws-a-case-study-20e6</t>
+        </is>
+      </c>
+      <c r="E154" s="5" t="n">
+        <v>45817.45672453703</v>
+      </c>
+      <c r="F154" s="4" t="inlineStr">
+        <is>
+          <t>#ai, #aws, #machinelearning, #tts</t>
+        </is>
+      </c>
+      <c r="G154" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H154" s="4" t="inlineStr"/>
+      <c r="I154" s="5" t="n">
+        <v>45817.55414351852</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="4" t="n">
+        <v>730</v>
+      </c>
+      <c r="B155" s="4" t="inlineStr">
+        <is>
+          <t>Day 12 - Component Fundamentals with JavaScript Frameworks</t>
+        </is>
+      </c>
+      <c r="C155" s="4" t="inlineStr">
+        <is>
+          <t>Connie Leung</t>
+        </is>
+      </c>
+      <c r="D155" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/railsstudent/day-12-component-fundamentals-with-javascript-frameworks-36dn</t>
+        </is>
+      </c>
+      <c r="E155" s="5" t="n">
+        <v>45817.4630787037</v>
+      </c>
+      <c r="F155" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #vue, #svelte, #angular</t>
+        </is>
+      </c>
+      <c r="G155" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H155" s="4" t="inlineStr"/>
+      <c r="I155" s="5" t="n">
+        <v>45817.56011574074</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="4" t="n">
+        <v>738</v>
+      </c>
+      <c r="B156" s="4" t="inlineStr">
+        <is>
+          <t>Stop What You're Doing: Angular 20's New Superpowers Will Change How You Code Forever</t>
+        </is>
+      </c>
+      <c r="C156" s="4" t="inlineStr">
+        <is>
+          <t>Rajat</t>
+        </is>
+      </c>
+      <c r="D156" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/codewithrajat/stop-what-youre-doing-angular-20s-new-superpowers-will-change-how-you-code-forever-54n6</t>
+        </is>
+      </c>
+      <c r="E156" s="5" t="n">
+        <v>45817.4630787037</v>
+      </c>
+      <c r="F156" s="4" t="inlineStr">
+        <is>
+          <t>#discuss, #programming, #webdev, #javascript</t>
+        </is>
+      </c>
+      <c r="G156" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" s="4" t="inlineStr"/>
+      <c r="I156" s="5" t="n">
+        <v>45817.58333333334</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="4" t="n">
+        <v>739</v>
+      </c>
+      <c r="B157" s="4" t="inlineStr">
+        <is>
+          <t>Je cherche un développeur pour s’entraîner sur un projet réel</t>
+        </is>
+      </c>
+      <c r="C157" s="4" t="inlineStr">
+        <is>
+          <t>P-thon</t>
+        </is>
+      </c>
+      <c r="D157" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/pthon/je-cherche-un-developpeur-pour-sentrainer-sur-un-projet-reel-5c7f</t>
+        </is>
+      </c>
+      <c r="E157" s="5" t="n">
+        <v>45817.4630787037</v>
+      </c>
+      <c r="F157" s="4" t="inlineStr">
+        <is>
+          <t>#beginners, #api, #design, #django</t>
+        </is>
+      </c>
+      <c r="G157" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="4" t="inlineStr"/>
+      <c r="I157" s="5" t="n">
+        <v>45817.58075231482</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="4" t="n">
+        <v>740</v>
+      </c>
+      <c r="B158" s="4" t="inlineStr">
+        <is>
+          <t>I Used AI to Debug My Code and Here's What Happened (Spoiler: Mind = Blown 🤯)</t>
+        </is>
+      </c>
+      <c r="C158" s="4" t="inlineStr">
+        <is>
+          <t>faheem ismail</t>
+        </is>
+      </c>
+      <c r="D158" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/faheem_ismail_70074f405e7/i-used-ai-to-debug-my-code-and-heres-what-happened-spoiler-mind-blown--d42</t>
+        </is>
+      </c>
+      <c r="E158" s="5" t="n">
+        <v>45817.4630787037</v>
+      </c>
+      <c r="F158" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #programming, #javascript, #ai</t>
+        </is>
+      </c>
+      <c r="G158" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H158" s="4" t="inlineStr"/>
+      <c r="I158" s="5" t="n">
+        <v>45817.57928240741</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="4" t="n">
+        <v>750</v>
+      </c>
+      <c r="B159" s="4" t="inlineStr">
+        <is>
+          <t>Build an AI Meeting Assistant with Stream Video and LLMs</t>
+        </is>
+      </c>
+      <c r="C159" s="4" t="inlineStr">
+        <is>
+          <t>Quincy Oghenetejiri</t>
+        </is>
+      </c>
+      <c r="D159" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/getstreamhq/build-an-ai-meeting-assistant-with-stream-video-and-llms-4kah</t>
+        </is>
+      </c>
+      <c r="E159" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F159" s="4" t="inlineStr">
+        <is>
+          <t>#ai, #meeting, #programming, #productivity</t>
+        </is>
+      </c>
+      <c r="G159" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="H159" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I159" s="5" t="n">
+        <v>45817.59390046296</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="4" t="n">
+        <v>752</v>
+      </c>
+      <c r="B160" s="4" t="inlineStr">
+        <is>
+          <t>Tidbit 03: innerText vs textContent in JavaScript – Not Twins, Just Cousins!</t>
+        </is>
+      </c>
+      <c r="C160" s="4" t="inlineStr">
+        <is>
+          <t>Tapas Adhikary</t>
+        </is>
+      </c>
+      <c r="D160" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/atapas/tidbit-03-innertext-vs-textcontent-in-javascript-not-twins-just-cousins-3i4a</t>
+        </is>
+      </c>
+      <c r="E160" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F160" s="4" t="inlineStr">
+        <is>
+          <t>#webdev, #javascript, #programming, #codenewbie</t>
+        </is>
+      </c>
+      <c r="G160" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" s="4" t="inlineStr"/>
+      <c r="I160" s="5" t="n">
+        <v>45817.59513888889</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="4" t="n">
+        <v>758</v>
+      </c>
+      <c r="B161" s="4" t="inlineStr">
+        <is>
+          <t>How to connect Supabase to Microsoft Power BI</t>
+        </is>
+      </c>
+      <c r="C161" s="4" t="inlineStr">
+        <is>
+          <t>jenny</t>
+        </is>
+      </c>
+      <c r="D161" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/jenniekibiri/how-to-connect-supabase-to-microsoft-power-bi-50p8</t>
+        </is>
+      </c>
+      <c r="E161" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F161" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G161" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H161" s="4" t="inlineStr"/>
+      <c r="I161" s="5" t="n">
+        <v>45817.5741087963</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="4" t="n">
+        <v>760</v>
+      </c>
+      <c r="B162" s="4" t="inlineStr">
+        <is>
+          <t>7 Strategies to Stay Sane in the Never-Ending Tech Hype Cycle</t>
+        </is>
+      </c>
+      <c r="C162" s="4" t="inlineStr">
+        <is>
+          <t>Cesar Aguirre</t>
+        </is>
+      </c>
+      <c r="D162" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/canro91/7-strategies-to-stay-sane-in-the-never-ending-tech-hype-cycle-3ef3</t>
+        </is>
+      </c>
+      <c r="E162" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F162" s="4" t="inlineStr">
+        <is>
+          <t>#discuss, #ai, #beginners, #programming</t>
+        </is>
+      </c>
+      <c r="G162" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H162" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I162" s="5" t="n">
+        <v>45817.20833333334</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="4" t="n">
+        <v>762</v>
+      </c>
+      <c r="B163" s="4" t="inlineStr">
+        <is>
+          <t>What are tracking pixels and how do they work?</t>
+        </is>
+      </c>
+      <c r="C163" s="4" t="inlineStr">
+        <is>
+          <t>Mehul Lakhanpal</t>
+        </is>
+      </c>
+      <c r="D163" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/ml318097/what-are-tracking-pixels-and-how-do-they-work-2pfe</t>
+        </is>
+      </c>
+      <c r="E163" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F163" s="4" t="inlineStr">
+        <is>
+          <t>#marketing, #webdev</t>
+        </is>
+      </c>
+      <c r="G163" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H163" s="4" t="inlineStr"/>
+      <c r="I163" s="5" t="n">
+        <v>45817.58604166667</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="4" t="n">
+        <v>765</v>
+      </c>
+      <c r="B164" s="4" t="inlineStr">
+        <is>
+          <t>Orchestrating Multi-User Workflows in Phoenix LiveView with WebSockets</t>
+        </is>
+      </c>
+      <c r="C164" s="4" t="inlineStr">
+        <is>
+          <t>HexShift</t>
+        </is>
+      </c>
+      <c r="D164" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/hexshift/orchestrating-multi-user-workflows-in-phoenix-liveview-with-websockets-g8d</t>
+        </is>
+      </c>
+      <c r="E164" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F164" s="4" t="inlineStr">
+        <is>
+          <t>#websockets, #elixir, #webdev</t>
+        </is>
+      </c>
+      <c r="G164" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H164" s="4" t="inlineStr"/>
+      <c r="I164" s="5" t="n">
+        <v>45817.60390046296</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="4" t="n">
+        <v>767</v>
+      </c>
+      <c r="B165" s="4" t="inlineStr">
+        <is>
+          <t>Reducing props size in Sitecore XM Cloud Next.js to improve performance</t>
+        </is>
+      </c>
+      <c r="C165" s="4" t="inlineStr">
+        <is>
+          <t>Sebastián Aliaga</t>
+        </is>
+      </c>
+      <c r="D165" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/sebasab/reducing-props-size-in-sitecore-xm-cloud-nextjs-to-improve-performance-1850</t>
+        </is>
+      </c>
+      <c r="E165" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F165" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G165" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H165" s="4" t="inlineStr"/>
+      <c r="I165" s="5" t="n">
+        <v>45817.59672453703</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="4" t="n">
+        <v>770</v>
+      </c>
+      <c r="B166" s="4" t="inlineStr">
+        <is>
+          <t>How to Use Google Patents vs. PatentScan for Prior Art Searches: A Guide for IP Professionals</t>
+        </is>
+      </c>
+      <c r="C166" s="4" t="inlineStr">
+        <is>
+          <t>Zainab Imran</t>
+        </is>
+      </c>
+      <c r="D166" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/patentscanai/how-to-use-google-patents-vs-patentscan-for-prior-art-searches-a-guide-for-ip-professionals-5e95</t>
+        </is>
+      </c>
+      <c r="E166" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F166" s="4" t="inlineStr">
+        <is>
+          <t>#techtalks, #ai, #patentanalysis, #beginners</t>
+        </is>
+      </c>
+      <c r="G166" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H166" s="4" t="inlineStr"/>
+      <c r="I166" s="5" t="n">
+        <v>45817.58251157407</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="4" t="n">
+        <v>771</v>
+      </c>
+      <c r="B167" s="4" t="inlineStr">
+        <is>
+          <t>DevOps What is DevSecOps? A guide to secure software development</t>
+        </is>
+      </c>
+      <c r="C167" s="4" t="inlineStr">
+        <is>
+          <t>Gatling.io</t>
+        </is>
+      </c>
+      <c r="D167" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/gatling/devopswhat-is-devsecops-a-guide-to-secure-software-development-5b60</t>
+        </is>
+      </c>
+      <c r="E167" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F167" s="4" t="inlineStr">
+        <is>
+          <t>#devops, #devsecops, #gatling</t>
+        </is>
+      </c>
+      <c r="G167" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" s="4" t="inlineStr"/>
+      <c r="I167" s="5" t="n">
+        <v>45817.58282407407</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="4" t="n">
+        <v>772</v>
+      </c>
+      <c r="B168" s="4" t="inlineStr">
+        <is>
+          <t>Elasticsearch Indexing Strategies</t>
+        </is>
+      </c>
+      <c r="C168" s="4" t="inlineStr">
+        <is>
+          <t>Akshat Jaiswal</t>
+        </is>
+      </c>
+      <c r="D168" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/akshat-ast/elasticsearch-indexing-strategies-54o7</t>
+        </is>
+      </c>
+      <c r="E168" s="5" t="n">
+        <v>45817.48804398148</v>
+      </c>
+      <c r="F168" s="4" t="inlineStr">
+        <is>
+          <t>#elasticsearch, #indexing, #astconsulting, #backenddevelopment</t>
+        </is>
+      </c>
+      <c r="G168" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H168" s="4" t="inlineStr"/>
+      <c r="I168" s="5" t="n">
+        <v>45817.57659722222</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="4" t="n">
+        <v>792</v>
+      </c>
+      <c r="B169" s="4" t="inlineStr">
+        <is>
+          <t>Today I learned-JavaScript: while Loops, Arrow Functions, and the map() Method</t>
+        </is>
+      </c>
+      <c r="C169" s="4" t="inlineStr">
+        <is>
+          <t>P Mukila</t>
+        </is>
+      </c>
+      <c r="D169" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/mukilaperiyasamy/today-i-learned-javascript-while-loops-arrow-functions-and-the-map-method-41d1</t>
+        </is>
+      </c>
+      <c r="E169" s="5" t="n">
+        <v>45817.49130787037</v>
+      </c>
+      <c r="F169" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G169" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H169" s="4" t="inlineStr"/>
+      <c r="I169" s="5" t="n">
+        <v>45817.60578703704</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="4" t="n">
+        <v>793</v>
+      </c>
+      <c r="B170" s="4" t="inlineStr">
+        <is>
+          <t>Tutorial on the Implementation of Picker Date Picker</t>
+        </is>
+      </c>
+      <c r="C170" s="4" t="inlineStr">
+        <is>
+          <t>liu yang</t>
+        </is>
+      </c>
+      <c r="D170" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/liu_yang_fc0e605820ac220c/tutorial-on-the-implementation-of-picker-date-picker-15nh</t>
+        </is>
+      </c>
+      <c r="E170" s="5" t="n">
+        <v>45817.49130787037</v>
+      </c>
+      <c r="F170" s="4" t="inlineStr">
+        <is>
+          <t>#harmonyosnext</t>
+        </is>
+      </c>
+      <c r="G170" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H170" s="4" t="inlineStr"/>
+      <c r="I170" s="5" t="n">
+        <v>45817.60712962963</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="4" t="n">
+        <v>794</v>
+      </c>
+      <c r="B171" s="4" t="inlineStr">
+        <is>
+          <t>The Role of Data Warehousing and Dimensional Modeling in Building a Scalable Data Warehouse for AI Agents</t>
+        </is>
+      </c>
+      <c r="C171" s="4" t="inlineStr">
+        <is>
+          <t>Bob Otieno Okech</t>
+        </is>
+      </c>
+      <c r="D171" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/bobokech/the-role-of-data-warehousing-and-dimensional-modeling-in-building-a-scalable-data-warehouse-for-ai-2nek</t>
+        </is>
+      </c>
+      <c r="E171" s="5" t="n">
+        <v>45817.49130787037</v>
+      </c>
+      <c r="F171" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G171" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H171" s="4" t="inlineStr"/>
+      <c r="I171" s="5" t="n">
+        <v>45817.60946759259</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="4" t="n">
+        <v>795</v>
+      </c>
+      <c r="B172" s="4" t="inlineStr">
+        <is>
+          <t># 🔁 JavaScript Essentials: While Loops, Arrow Functions &amp; the Map Method.</t>
+        </is>
+      </c>
+      <c r="C172" s="4" t="inlineStr">
+        <is>
+          <t>rajeshwari rajeshwari</t>
+        </is>
+      </c>
+      <c r="D172" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/rajeshwari_rajeshwari_0e5/-javascript-essentials-while-loops-arrow-functions-the-map-method-2akg</t>
+        </is>
+      </c>
+      <c r="E172" s="5" t="n">
+        <v>45817.49130787037</v>
+      </c>
+      <c r="F172" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G172" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H172" s="4" t="inlineStr"/>
+      <c r="I172" s="5" t="n">
+        <v>45817.60613425926</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="4" t="n">
+        <v>796</v>
+      </c>
+      <c r="B173" s="4" t="inlineStr">
+        <is>
+          <t>JavaScript Essentials: While Loop, Map Function &amp; Arrow Functions</t>
+        </is>
+      </c>
+      <c r="C173" s="4" t="inlineStr">
+        <is>
+          <t>kanaga vimala</t>
+        </is>
+      </c>
+      <c r="D173" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/kanaga_vimala_66acce9cf6e/javascript-essentials-while-loop-map-function-arrow-functions-3462</t>
+        </is>
+      </c>
+      <c r="E173" s="5" t="n">
+        <v>45817.49130787037</v>
+      </c>
+      <c r="F173" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G173" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H173" s="4" t="inlineStr"/>
+      <c r="I173" s="5" t="n">
+        <v>45817.61075231482</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="4" t="n">
+        <v>840</v>
+      </c>
+      <c r="B174" s="4" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈 Pride RS: LGBTQ+ Flag Component for Rust Frontends</t>
+        </is>
+      </c>
+      <c r="C174" s="4" t="inlineStr">
+        <is>
+          <t>Mahmoud Harmouch</t>
+        </is>
+      </c>
+      <c r="D174" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/wiseai/pride-rs-lgbtq-flag-component-for-rust-frontends-1e60</t>
+        </is>
+      </c>
+      <c r="E174" s="5" t="n">
+        <v>45817.49956018518</v>
+      </c>
+      <c r="F174" s="4" t="inlineStr">
+        <is>
+          <t>#frontendchallenge, #devchallenge, #css, #rust</t>
+        </is>
+      </c>
+      <c r="G174" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H174" s="4" t="inlineStr"/>
+      <c r="I174" s="5" t="n">
+        <v>45817.61817129629</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="4" t="n">
+        <v>841</v>
+      </c>
+      <c r="B175" s="4" t="inlineStr">
+        <is>
+          <t>Embarking Your Laravel Journey: A Beginner's Soulful Guide to Crafting Web Magic</t>
+        </is>
+      </c>
+      <c r="C175" s="4" t="inlineStr">
+        <is>
+          <t>Coder</t>
+        </is>
+      </c>
+      <c r="D175" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/vaib/embarking-your-laravel-journey-a-beginners-soulful-guide-to-crafting-web-magic-34gj</t>
+        </is>
+      </c>
+      <c r="E175" s="5" t="n">
+        <v>45817.49956018518</v>
+      </c>
+      <c r="F175" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G175" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H175" s="4" t="inlineStr"/>
+      <c r="I175" s="5" t="n">
+        <v>45817.61489583334</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="4" t="n">
+        <v>842</v>
+      </c>
+      <c r="B176" s="4" t="inlineStr">
+        <is>
+          <t>🚀 17 and Full-Stack: My Dev Journey So Far</t>
+        </is>
+      </c>
+      <c r="C176" s="4" t="inlineStr">
+        <is>
+          <t>Rvn</t>
+        </is>
+      </c>
+      <c r="D176" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/00rvn00/17-and-full-stack-my-dev-journey-so-far-1499</t>
+        </is>
+      </c>
+      <c r="E176" s="5" t="n">
+        <v>45817.49956018518</v>
+      </c>
+      <c r="F176" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G176" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H176" s="4" t="inlineStr"/>
+      <c r="I176" s="5" t="n">
+        <v>45817.61697916667</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="4" t="n">
+        <v>843</v>
+      </c>
+      <c r="B177" s="4" t="inlineStr">
+        <is>
+          <t>The Ethics of Artificial Intelligence</t>
+        </is>
+      </c>
+      <c r="C177" s="4" t="inlineStr">
+        <is>
+          <t>Ritesh Kokam</t>
+        </is>
+      </c>
+      <c r="D177" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/riteshkokam/the-ethics-of-artificial-intelligence-3e17</t>
+        </is>
+      </c>
+      <c r="E177" s="5" t="n">
+        <v>45817.49956018518</v>
+      </c>
+      <c r="F177" s="4" t="inlineStr">
+        <is>
+          <t>#programming, #ai, #learning, #machinelearning</t>
+        </is>
+      </c>
+      <c r="G177" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H177" s="4" t="inlineStr"/>
+      <c r="I177" s="5" t="n">
+        <v>45817.61609953704</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="4" t="n">
+        <v>845</v>
+      </c>
+      <c r="B178" s="4" t="inlineStr">
+        <is>
+          <t>💡 Why I’m Building RelayBeam - Fixing the Gaps in How We Communicate Today</t>
+        </is>
+      </c>
+      <c r="C178" s="4" t="inlineStr">
+        <is>
+          <t>Suprit Gandhi</t>
+        </is>
+      </c>
+      <c r="D178" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/supritgandhi/why-im-building-relaybeam-fixing-the-gaps-in-how-we-communicate-today-5li</t>
+        </is>
+      </c>
+      <c r="E178" s="5" t="n">
+        <v>45817.49956018518</v>
+      </c>
+      <c r="F178" s="4" t="inlineStr">
+        <is>
+          <t>#startup, #webdev, #javascript, #productivity</t>
+        </is>
+      </c>
+      <c r="G178" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H178" s="4" t="inlineStr"/>
+      <c r="I178" s="5" t="n">
+        <v>45817.59998842593</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="4" t="n">
+        <v>942</v>
+      </c>
+      <c r="B179" s="4" t="inlineStr">
+        <is>
+          <t>Level 1 Unreal Engine</t>
+        </is>
+      </c>
+      <c r="C179" s="4" t="inlineStr">
+        <is>
+          <t>Charlie Perry</t>
+        </is>
+      </c>
+      <c r="D179" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/charlie_perry_e1d44dc7773/level-1-unreal-engine-4f9b</t>
+        </is>
+      </c>
+      <c r="E179" s="5" t="n">
+        <v>45817.5128587963</v>
+      </c>
+      <c r="F179" s="4" t="inlineStr">
+        <is>
+          <t>#gamedev, #leveldesign, #unrealengine</t>
+        </is>
+      </c>
+      <c r="G179" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H179" s="4" t="inlineStr"/>
+      <c r="I179" s="5" t="n">
+        <v>45817.6279050926</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="4" t="n">
+        <v>943</v>
+      </c>
+      <c r="B180" s="4" t="inlineStr">
+        <is>
+          <t>What I Learned by Looking Outside</t>
+        </is>
+      </c>
+      <c r="C180" s="4" t="inlineStr">
+        <is>
+          <t>Tommy Nguyen</t>
+        </is>
+      </c>
+      <c r="D180" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/tuannvm/what-i-learned-by-looking-outside-59ep</t>
+        </is>
+      </c>
+      <c r="E180" s="5" t="n">
+        <v>45817.5128587963</v>
+      </c>
+      <c r="F180" s="4" t="inlineStr">
+        <is>
+          <t>Sem tags</t>
+        </is>
+      </c>
+      <c r="G180" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H180" s="4" t="inlineStr"/>
+      <c r="I180" s="5" t="n">
+        <v>45817.63217592592</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="4" t="n">
+        <v>944</v>
+      </c>
+      <c r="B181" s="4" t="inlineStr">
+        <is>
+          <t>Day 31 - Day 32: Landing</t>
+        </is>
+      </c>
+      <c r="C181" s="4" t="inlineStr">
+        <is>
+          <t>Edward Chia</t>
+        </is>
+      </c>
+      <c r="D181" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/edwardcjianken/day-31-day-32-landing-49gd</t>
+        </is>
+      </c>
+      <c r="E181" s="5" t="n">
+        <v>45817.5128587963</v>
+      </c>
+      <c r="F181" s="4" t="inlineStr">
+        <is>
+          <t>#100daysofcode, #devjournal, #frontend</t>
+        </is>
+      </c>
+      <c r="G181" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H181" s="4" t="inlineStr"/>
+      <c r="I181" s="5" t="n">
+        <v>45817.62810185185</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="4" t="n">
+        <v>1013</v>
+      </c>
+      <c r="B182" s="4" t="inlineStr">
+        <is>
+          <t>Symfony and MongoDB: Our Commitment to a Stronger Integration</t>
+        </is>
+      </c>
+      <c r="C182" s="4" t="inlineStr">
+        <is>
+          <t>MongoDB Guests</t>
+        </is>
+      </c>
+      <c r="D182" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/mongodb/symfony-and-mongodb-our-commitment-to-a-stronger-integration-hf4</t>
+        </is>
+      </c>
+      <c r="E182" s="5" t="n">
+        <v>45817.5203125</v>
+      </c>
+      <c r="F182" s="4" t="inlineStr">
+        <is>
+          <t>#symfony, #mongodb, #webdev, #programming</t>
+        </is>
+      </c>
+      <c r="G182" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H182" s="4" t="inlineStr"/>
+      <c r="I182" s="5" t="n">
+        <v>45817.63297453704</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="4" t="n">
+        <v>1016</v>
+      </c>
+      <c r="B183" s="4" t="inlineStr">
+        <is>
+          <t>Clear and well-explained. The legal structure side of tech projects is something we don’t talk about enough and this nailed it.</t>
+        </is>
+      </c>
+      <c r="C183" s="4" t="inlineStr">
+        <is>
+          <t>Celeste Hargrove</t>
+        </is>
+      </c>
+      <c r="D183" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/celestehar88/clear-and-well-explained-the-legal-structure-side-of-tech-projects-is-something-we-dont-talk-41i7</t>
+        </is>
+      </c>
+      <c r="E183" s="5" t="n">
+        <v>45817.5203125</v>
+      </c>
+      <c r="F183" s="4" t="inlineStr">
+        <is>
+          <t>#startup, #devtools, #tdzpro, #entrepreneurship</t>
+        </is>
+      </c>
+      <c r="G183" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H183" s="4" t="inlineStr"/>
+      <c r="I183" s="5" t="n">
+        <v>45817.6334375</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="4" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B184" s="4" t="inlineStr">
+        <is>
+          <t>🚀 Streamline Your Python &amp; Django Development with Production-Ready Cookiecutter Templates</t>
+        </is>
+      </c>
+      <c r="C184" s="4" t="inlineStr">
+        <is>
+          <t>Huy Nguyen</t>
+        </is>
+      </c>
+      <c r="D184" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/huynguyengl99/streamline-your-python-django-development-with-production-ready-cookiecutter-templates-455o</t>
+        </is>
+      </c>
+      <c r="E184" s="5" t="n">
+        <v>45817.5203125</v>
+      </c>
+      <c r="F184" s="4" t="inlineStr">
+        <is>
+          <t>#python, #cookiecutter, #bestpractices, #devtools</t>
+        </is>
+      </c>
+      <c r="G184" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H184" s="4" t="inlineStr"/>
+      <c r="I184" s="5" t="n">
+        <v>45817.63811342593</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="4" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B185" s="4" t="inlineStr">
+        <is>
+          <t>QuCode - 21DaysChallenge - Day 08</t>
+        </is>
+      </c>
+      <c r="C185" s="4" t="inlineStr">
+        <is>
+          <t>Paulo B.M. Sousa</t>
+        </is>
+      </c>
+      <c r="D185" s="4" t="inlineStr">
+        <is>
+          <t>https://dev.to/paulobmsousa/qucode-21dayschallenge-day-08-20ni</t>
+        </is>
+      </c>
+      <c r="E185" s="5" t="n">
+        <v>45817.5203125</v>
+      </c>
+      <c r="F185" s="4" t="inlineStr">
+        <is>
+          <t>#quantum, #python, #codenewbie, #tutorial</t>
+        </is>
+      </c>
+      <c r="G185" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H185" s="4" t="inlineStr"/>
+      <c r="I185" s="5" t="n">
+        <v>45817.63680555556</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I130"/>
+  <autoFilter ref="A1:I185"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>